<commit_message>
excel input mapped to output (same attr copy)
</commit_message>
<xml_diff>
--- a/uploads/output.xlsx
+++ b/uploads/output.xlsx
@@ -375,35 +375,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:EA2"/>
+  <dimension ref="A1:FH6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>0</v>
+        <v>last name</v>
       </c>
       <c r="B1" t="str">
-        <v>last name</v>
+        <v>first name</v>
       </c>
       <c r="C1" t="str">
-        <v>first name</v>
+        <v>other names currently or previously used</v>
       </c>
       <c r="D1" t="str">
-        <v>other names currently or previously used</v>
+        <v>dob</v>
       </c>
       <c r="E1" t="str">
-        <v>dob</v>
+        <v>ssn</v>
       </c>
       <c r="F1" t="str">
-        <v>ssn</v>
+        <v>field of practice</v>
       </c>
       <c r="G1" t="str">
-        <v>field of practice</v>
+        <v>npi number on application</v>
       </c>
       <c r="H1" t="str">
-        <v>npi number on application</v>
+        <v xml:space="preserve"> npi- dentists full name</v>
       </c>
       <c r="I1" t="str">
         <v>i do not precribe controlled substances</v>
@@ -415,372 +415,474 @@
         <v>dea number from application</v>
       </c>
       <c r="L1" t="str">
+        <v>dea name (company name)</v>
+      </c>
+      <c r="M1" t="str">
+        <v>dea state</v>
+      </c>
+      <c r="N1" t="str">
+        <v>dea expiration date</v>
+      </c>
+      <c r="O1" t="str">
+        <v>dea verified date</v>
+      </c>
+      <c r="P1" t="str">
+        <v>oig</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>oig verified date</v>
+      </c>
+      <c r="R1" t="str">
+        <v>is name on do not recruit list</v>
+      </c>
+      <c r="S1" t="str">
+        <v>is npi on do not recruit list</v>
+      </c>
+      <c r="T1" t="str">
         <v>state license number from application</v>
       </c>
-      <c r="M1" t="str">
+      <c r="U1" t="str">
         <v>state license state from application</v>
       </c>
-      <c r="N1" t="str">
+      <c r="V1" t="str">
+        <v>name on state license</v>
+      </c>
+      <c r="W1" t="str">
+        <v>expiration date</v>
+      </c>
+      <c r="X1" t="str">
+        <v>status</v>
+      </c>
+      <c r="Y1" t="str">
+        <v>discipline indicator</v>
+      </c>
+      <c r="Z1" t="str">
+        <v>verified date</v>
+      </c>
+      <c r="AA1" t="str">
         <v>state license number from application_1</v>
       </c>
-      <c r="O1" t="str">
+      <c r="AB1" t="str">
         <v>state license state from application_1</v>
       </c>
-      <c r="P1" t="str">
+      <c r="AC1" t="str">
+        <v>name on state license_1</v>
+      </c>
+      <c r="AD1" t="str">
+        <v>expiration date_1</v>
+      </c>
+      <c r="AE1" t="str">
+        <v>status_1</v>
+      </c>
+      <c r="AF1" t="str">
+        <v>discipline indicator_1</v>
+      </c>
+      <c r="AG1" t="str">
+        <v>verified date_1</v>
+      </c>
+      <c r="AH1" t="str">
         <v>state license number from application_2</v>
       </c>
-      <c r="Q1" t="str">
+      <c r="AI1" t="str">
         <v>state license state from application_2</v>
       </c>
-      <c r="R1" t="str">
+      <c r="AJ1" t="str">
+        <v>name on state license_2</v>
+      </c>
+      <c r="AK1" t="str">
+        <v>expiration date_2</v>
+      </c>
+      <c r="AL1" t="str">
+        <v>status_2</v>
+      </c>
+      <c r="AM1" t="str">
+        <v>discipline indicator_2</v>
+      </c>
+      <c r="AN1" t="str">
+        <v>verified date_2</v>
+      </c>
+      <c r="AO1" t="str">
         <v>address from application</v>
       </c>
-      <c r="S1" t="str">
+      <c r="AP1" t="str">
         <v>location start date</v>
       </c>
-      <c r="T1" t="str">
+      <c r="AQ1" t="str">
         <v>street</v>
       </c>
-      <c r="U1" t="str">
+      <c r="AR1" t="str">
         <v>city</v>
       </c>
-      <c r="V1" t="str">
+      <c r="AS1" t="str">
         <v>state</v>
       </c>
-      <c r="W1" t="str">
+      <c r="AT1" t="str">
         <v>zip</v>
       </c>
-      <c r="X1" t="str">
+      <c r="AU1" t="str">
         <v>tin</v>
       </c>
-      <c r="Y1" t="str">
+      <c r="AV1" t="str">
+        <v>is tin on do not recruit list yes or no</v>
+      </c>
+      <c r="AW1" t="str">
         <v>address from application_1</v>
       </c>
-      <c r="Z1" t="str">
+      <c r="AX1" t="str">
         <v>location start date_1</v>
       </c>
-      <c r="AA1" t="str">
+      <c r="AY1" t="str">
         <v>street_1</v>
       </c>
-      <c r="AB1" t="str">
+      <c r="AZ1" t="str">
         <v>city_1</v>
       </c>
-      <c r="AC1" t="str">
+      <c r="BA1" t="str">
         <v>state_1</v>
       </c>
-      <c r="AD1" t="str">
+      <c r="BB1" t="str">
         <v>zip_1</v>
       </c>
-      <c r="AE1" t="str">
+      <c r="BC1" t="str">
         <v>tin_1</v>
       </c>
-      <c r="AF1" t="str">
+      <c r="BD1" t="str">
+        <v>is tin on do not recruit list yes or no_1</v>
+      </c>
+      <c r="BE1" t="str">
         <v>address from application_2</v>
       </c>
-      <c r="AG1" t="str">
+      <c r="BF1" t="str">
         <v>location start date_2</v>
       </c>
-      <c r="AH1" t="str">
+      <c r="BG1" t="str">
         <v>street_2</v>
       </c>
-      <c r="AI1" t="str">
+      <c r="BH1" t="str">
         <v>city_2</v>
       </c>
-      <c r="AJ1" t="str">
+      <c r="BI1" t="str">
         <v>state_2</v>
       </c>
-      <c r="AK1" t="str">
+      <c r="BJ1" t="str">
         <v>zip_2</v>
       </c>
-      <c r="AL1" t="str">
+      <c r="BK1" t="str">
         <v>tin_2</v>
       </c>
-      <c r="AM1" t="str">
+      <c r="BL1" t="str">
+        <v>is tin on do not recruit list yes or no_2</v>
+      </c>
+      <c r="BM1" t="str">
         <v>address from application_3</v>
       </c>
-      <c r="AN1" t="str">
+      <c r="BN1" t="str">
         <v>location start date_3</v>
       </c>
-      <c r="AO1" t="str">
+      <c r="BO1" t="str">
         <v>street_3</v>
       </c>
-      <c r="AP1" t="str">
+      <c r="BP1" t="str">
         <v>city_3</v>
       </c>
-      <c r="AQ1" t="str">
+      <c r="BQ1" t="str">
         <v>state_3</v>
       </c>
-      <c r="AR1" t="str">
+      <c r="BR1" t="str">
         <v>zip_3</v>
       </c>
-      <c r="AS1" t="str">
+      <c r="BS1" t="str">
         <v>tin_3</v>
       </c>
-      <c r="AT1" t="str">
+      <c r="BT1" t="str">
+        <v>is tin on do not recruit list yes or no_3</v>
+      </c>
+      <c r="BU1" t="str">
         <v>address from application_4</v>
       </c>
-      <c r="AU1" t="str">
+      <c r="BV1" t="str">
         <v>location start date_4</v>
       </c>
-      <c r="AV1" t="str">
+      <c r="BW1" t="str">
         <v>street_4</v>
       </c>
-      <c r="AW1" t="str">
+      <c r="BX1" t="str">
         <v>city_4</v>
       </c>
-      <c r="AX1" t="str">
+      <c r="BY1" t="str">
         <v>state_4</v>
       </c>
-      <c r="AY1" t="str">
+      <c r="BZ1" t="str">
         <v>zip_4</v>
       </c>
-      <c r="AZ1" t="str">
+      <c r="CA1" t="str">
         <v>tin_4</v>
       </c>
-      <c r="BA1" t="str">
+      <c r="CB1" t="str">
+        <v>is tin on do not recruit list yes or no_4</v>
+      </c>
+      <c r="CC1" t="str">
         <v>address from application_5</v>
       </c>
-      <c r="BB1" t="str">
+      <c r="CD1" t="str">
         <v>location start date_5</v>
       </c>
-      <c r="BC1" t="str">
+      <c r="CE1" t="str">
         <v>street_5</v>
       </c>
-      <c r="BD1" t="str">
+      <c r="CF1" t="str">
         <v>city_5</v>
       </c>
-      <c r="BE1" t="str">
+      <c r="CG1" t="str">
         <v>state_5</v>
       </c>
-      <c r="BF1" t="str">
+      <c r="CH1" t="str">
         <v>zip_5</v>
       </c>
-      <c r="BG1" t="str">
+      <c r="CI1" t="str">
         <v>tin_5</v>
       </c>
-      <c r="BH1" t="str">
+      <c r="CJ1" t="str">
+        <v>is tin on do not recruit list yes or no_5</v>
+      </c>
+      <c r="CK1" t="str">
         <v>address from application_6</v>
       </c>
-      <c r="BI1" t="str">
+      <c r="CL1" t="str">
         <v>location start date_6</v>
       </c>
-      <c r="BJ1" t="str">
+      <c r="CM1" t="str">
         <v>street_6</v>
       </c>
-      <c r="BK1" t="str">
+      <c r="CN1" t="str">
         <v>city_6</v>
       </c>
-      <c r="BL1" t="str">
+      <c r="CO1" t="str">
         <v>state_6</v>
       </c>
-      <c r="BM1" t="str">
+      <c r="CP1" t="str">
         <v>zip_6</v>
       </c>
-      <c r="BN1" t="str">
+      <c r="CQ1" t="str">
         <v>tin_6</v>
       </c>
-      <c r="BO1" t="str">
+      <c r="CR1" t="str">
+        <v>is tin on do not recruit list yes or no_6</v>
+      </c>
+      <c r="CS1" t="str">
         <v>address from application_7</v>
       </c>
-      <c r="BP1" t="str">
+      <c r="CT1" t="str">
         <v>location start date_7</v>
       </c>
-      <c r="BQ1" t="str">
+      <c r="CU1" t="str">
         <v>street_7</v>
       </c>
-      <c r="BR1" t="str">
+      <c r="CV1" t="str">
         <v>city_7</v>
       </c>
-      <c r="BS1" t="str">
+      <c r="CW1" t="str">
         <v>state_7</v>
       </c>
-      <c r="BT1" t="str">
+      <c r="CX1" t="str">
         <v>zip_7</v>
       </c>
-      <c r="BU1" t="str">
+      <c r="CY1" t="str">
         <v>tin_7</v>
       </c>
-      <c r="BV1" t="str">
+      <c r="CZ1" t="str">
+        <v>is tin on do not recruit list yes or no_7</v>
+      </c>
+      <c r="DA1" t="str">
         <v>address from application_8</v>
       </c>
-      <c r="BW1" t="str">
+      <c r="DB1" t="str">
         <v>location start date_8</v>
       </c>
-      <c r="BX1" t="str">
+      <c r="DC1" t="str">
         <v>street_8</v>
       </c>
-      <c r="BY1" t="str">
+      <c r="DD1" t="str">
         <v>city_8</v>
       </c>
-      <c r="BZ1" t="str">
+      <c r="DE1" t="str">
         <v>state_8</v>
       </c>
-      <c r="CA1" t="str">
+      <c r="DF1" t="str">
         <v>zip_8</v>
       </c>
-      <c r="CB1" t="str">
+      <c r="DG1" t="str">
         <v>tin_8</v>
       </c>
-      <c r="CC1" t="str">
+      <c r="DH1" t="str">
+        <v>is tin on do not recruit list yes or no_8</v>
+      </c>
+      <c r="DI1" t="str">
         <v>address from application_9</v>
       </c>
-      <c r="CD1" t="str">
+      <c r="DJ1" t="str">
         <v>location start date_9</v>
       </c>
-      <c r="CE1" t="str">
+      <c r="DK1" t="str">
         <v>street_9</v>
       </c>
-      <c r="CF1" t="str">
+      <c r="DL1" t="str">
         <v>city_9</v>
       </c>
-      <c r="CG1" t="str">
+      <c r="DM1" t="str">
         <v>state_9</v>
       </c>
-      <c r="CH1" t="str">
+      <c r="DN1" t="str">
         <v>zip_9</v>
       </c>
-      <c r="CI1" t="str">
+      <c r="DO1" t="str">
         <v>tin_9</v>
       </c>
-      <c r="CJ1" t="str">
+      <c r="DP1" t="str">
+        <v>is tin on do not recruit list yes or no_9</v>
+      </c>
+      <c r="DQ1" t="str">
         <v>dentist's name</v>
       </c>
-      <c r="CK1" t="str">
+      <c r="DR1" t="str">
         <v>application signed date</v>
       </c>
-      <c r="CL1" t="str">
+      <c r="DS1" t="str">
         <v>application dentist's signature</v>
       </c>
-      <c r="CM1" t="str">
+      <c r="DT1" t="str">
         <v>license /confidential info: question 1 yes or no</v>
       </c>
-      <c r="CN1" t="str">
+      <c r="DU1" t="str">
         <v>license /confidential info: question 2 yes or no</v>
       </c>
-      <c r="CO1" t="str">
+      <c r="DV1" t="str">
         <v>license /confidential info: question 3 yes or no</v>
       </c>
-      <c r="CP1" t="str">
+      <c r="DW1" t="str">
         <v>license /confidential info: question 4 yes or no</v>
       </c>
-      <c r="CQ1" t="str">
+      <c r="DX1" t="str">
         <v>license /confidential info: question 5 yes or no</v>
       </c>
-      <c r="CR1" t="str">
+      <c r="DY1" t="str">
         <v>license /confidential info: question 6 yes or no</v>
       </c>
-      <c r="CS1" t="str">
+      <c r="DZ1" t="str">
         <v>license /confidential info: question 7 yes or no</v>
       </c>
-      <c r="CT1" t="str">
+      <c r="EA1" t="str">
         <v>license /confidential info: question 8 yes or no</v>
       </c>
-      <c r="CU1" t="str">
+      <c r="EB1" t="str">
         <v>license /confidential info: question 9 yes or no</v>
       </c>
-      <c r="CV1" t="str">
+      <c r="EC1" t="str">
         <v>license /confidential info: question 10 yes or no</v>
       </c>
-      <c r="CW1" t="str">
+      <c r="ED1" t="str">
         <v>dental school</v>
       </c>
-      <c r="CX1" t="str">
+      <c r="EE1" t="str">
         <v>month/year graduated (dental school)</v>
       </c>
-      <c r="CY1" t="str">
+      <c r="EF1" t="str">
         <v>specialty training institute</v>
       </c>
-      <c r="CZ1" t="str">
+      <c r="EG1" t="str">
         <v>month/year completed (specialty training)</v>
       </c>
-      <c r="DA1" t="str">
+      <c r="EH1" t="str">
         <v>board certified yes or no</v>
       </c>
-      <c r="DB1" t="str">
+      <c r="EI1" t="str">
         <v>do you have hospital privileges yes or no</v>
       </c>
-      <c r="DC1" t="str">
+      <c r="EJ1" t="str">
         <v>hospital name</v>
       </c>
-      <c r="DD1" t="str">
+      <c r="EK1" t="str">
         <v>phone number</v>
       </c>
-      <c r="DE1" t="str">
+      <c r="EL1" t="str">
         <v>address</v>
       </c>
-      <c r="DF1" t="str">
+      <c r="EM1" t="str">
         <v>city_10</v>
       </c>
-      <c r="DG1" t="str">
+      <c r="EN1" t="str">
         <v>state_10</v>
       </c>
-      <c r="DH1" t="str">
+      <c r="EO1" t="str">
         <v>zip_10</v>
       </c>
-      <c r="DI1" t="str">
+      <c r="EP1" t="str">
         <v>previous practice name</v>
       </c>
-      <c r="DJ1" t="str">
+      <c r="EQ1" t="str">
         <v>city_11</v>
       </c>
-      <c r="DK1" t="str">
+      <c r="ER1" t="str">
         <v>state_11</v>
       </c>
-      <c r="DL1" t="str">
+      <c r="ES1" t="str">
         <v>start date</v>
       </c>
-      <c r="DM1" t="str">
+      <c r="ET1" t="str">
         <v>end date</v>
       </c>
-      <c r="DN1" t="str">
+      <c r="EU1" t="str">
         <v>previous practice name_1</v>
       </c>
-      <c r="DO1" t="str">
+      <c r="EV1" t="str">
         <v>city_12</v>
       </c>
-      <c r="DP1" t="str">
+      <c r="EW1" t="str">
         <v>state_12</v>
       </c>
-      <c r="DQ1" t="str">
+      <c r="EX1" t="str">
         <v>start date_1</v>
       </c>
-      <c r="DR1" t="str">
+      <c r="EY1" t="str">
         <v>end date_1</v>
       </c>
-      <c r="DS1" t="str">
+      <c r="EZ1" t="str">
         <v>previous practice name_2</v>
       </c>
-      <c r="DT1" t="str">
+      <c r="FA1" t="str">
         <v>city_13</v>
       </c>
-      <c r="DU1" t="str">
+      <c r="FB1" t="str">
         <v>state_13</v>
       </c>
-      <c r="DV1" t="str">
+      <c r="FC1" t="str">
         <v>start date_2</v>
       </c>
-      <c r="DW1" t="str">
+      <c r="FD1" t="str">
         <v>end date_2</v>
       </c>
-      <c r="DX1" t="str">
+      <c r="FE1" t="str">
         <v>contact person name</v>
       </c>
-      <c r="DY1" t="str">
+      <c r="FF1" t="str">
         <v>phone</v>
       </c>
-      <c r="DZ1" t="str">
+      <c r="FG1" t="str">
         <v>email</v>
       </c>
-      <c r="EA1" t="str">
+      <c r="FH1" t="str">
         <v>dentist's email for correspondence</v>
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="str">
+        <v>Arak</v>
+      </c>
       <c r="B2" t="str">
-        <v>Arak</v>
+        <v>Marc</v>
       </c>
       <c r="C2" t="str">
-        <v>Marc</v>
+        <v>-</v>
       </c>
       <c r="D2" t="str">
         <v>-</v>
@@ -789,14 +891,14 @@
         <v>-</v>
       </c>
       <c r="F2" t="str">
-        <v>-</v>
-      </c>
-      <c r="G2" t="str">
         <v>Dentist</v>
       </c>
-      <c r="H2">
+      <c r="G2">
         <v>1790897486</v>
       </c>
+      <c r="H2" t="str">
+        <v>-</v>
+      </c>
       <c r="I2" t="str">
         <v>-</v>
       </c>
@@ -807,35 +909,35 @@
         <v>-</v>
       </c>
       <c r="L2" t="str">
+        <v>-</v>
+      </c>
+      <c r="M2" t="str">
+        <v>-</v>
+      </c>
+      <c r="N2" t="str">
+        <v>-</v>
+      </c>
+      <c r="O2" t="str">
+        <v>-</v>
+      </c>
+      <c r="P2" t="str">
+        <v>-</v>
+      </c>
+      <c r="Q2" t="str">
+        <v>-</v>
+      </c>
+      <c r="R2" t="str">
+        <v>-</v>
+      </c>
+      <c r="S2" t="str">
+        <v>-</v>
+      </c>
+      <c r="T2" t="str">
         <v>D02502</v>
       </c>
-      <c r="M2" t="str">
+      <c r="U2" t="str">
         <v>arizona</v>
       </c>
-      <c r="N2" t="str">
-        <v>-</v>
-      </c>
-      <c r="O2" t="str">
-        <v>-</v>
-      </c>
-      <c r="P2" t="str">
-        <v>-</v>
-      </c>
-      <c r="Q2" t="str">
-        <v>-</v>
-      </c>
-      <c r="R2" t="str">
-        <v>-</v>
-      </c>
-      <c r="S2" t="str">
-        <v>-</v>
-      </c>
-      <c r="T2" t="str">
-        <v>-</v>
-      </c>
-      <c r="U2" t="str">
-        <v>-</v>
-      </c>
       <c r="V2" t="str">
         <v>-</v>
       </c>
@@ -1035,141 +1137,2216 @@
         <v>-</v>
       </c>
       <c r="CJ2" t="str">
+        <v>-</v>
+      </c>
+      <c r="CK2" t="str">
+        <v>-</v>
+      </c>
+      <c r="CL2" t="str">
+        <v>-</v>
+      </c>
+      <c r="CM2" t="str">
+        <v>-</v>
+      </c>
+      <c r="CN2" t="str">
+        <v>-</v>
+      </c>
+      <c r="CO2" t="str">
+        <v>-</v>
+      </c>
+      <c r="CP2" t="str">
+        <v>-</v>
+      </c>
+      <c r="CQ2" t="str">
+        <v>-</v>
+      </c>
+      <c r="CR2" t="str">
+        <v>-</v>
+      </c>
+      <c r="CS2" t="str">
+        <v>-</v>
+      </c>
+      <c r="CT2" t="str">
+        <v>-</v>
+      </c>
+      <c r="CU2" t="str">
+        <v>-</v>
+      </c>
+      <c r="CV2" t="str">
+        <v>-</v>
+      </c>
+      <c r="CW2" t="str">
+        <v>-</v>
+      </c>
+      <c r="CX2" t="str">
+        <v>-</v>
+      </c>
+      <c r="CY2" t="str">
+        <v>-</v>
+      </c>
+      <c r="CZ2" t="str">
+        <v>-</v>
+      </c>
+      <c r="DA2" t="str">
+        <v>-</v>
+      </c>
+      <c r="DB2" t="str">
+        <v>-</v>
+      </c>
+      <c r="DC2" t="str">
+        <v>-</v>
+      </c>
+      <c r="DD2" t="str">
+        <v>-</v>
+      </c>
+      <c r="DE2" t="str">
+        <v>-</v>
+      </c>
+      <c r="DF2" t="str">
+        <v>-</v>
+      </c>
+      <c r="DG2" t="str">
+        <v>-</v>
+      </c>
+      <c r="DH2" t="str">
+        <v>-</v>
+      </c>
+      <c r="DI2" t="str">
+        <v>-</v>
+      </c>
+      <c r="DJ2" t="str">
+        <v>-</v>
+      </c>
+      <c r="DK2" t="str">
+        <v>-</v>
+      </c>
+      <c r="DL2" t="str">
+        <v>-</v>
+      </c>
+      <c r="DM2" t="str">
+        <v>-</v>
+      </c>
+      <c r="DN2" t="str">
+        <v>-</v>
+      </c>
+      <c r="DO2" t="str">
+        <v>-</v>
+      </c>
+      <c r="DP2" t="str">
+        <v>-</v>
+      </c>
+      <c r="DQ2" t="str">
         <v>Marc T. Arak</v>
       </c>
-      <c r="CK2">
+      <c r="DR2">
         <v>43893</v>
       </c>
-      <c r="CL2" t="str">
-        <v>-</v>
-      </c>
-      <c r="CM2" t="str">
+      <c r="DS2" t="str">
+        <v>-</v>
+      </c>
+      <c r="DT2" t="str">
         <v>yes</v>
       </c>
-      <c r="CN2" t="str">
+      <c r="DU2" t="str">
         <v>no</v>
       </c>
-      <c r="CO2" t="str">
+      <c r="DV2" t="str">
         <v>yes</v>
       </c>
-      <c r="CP2" t="str">
+      <c r="DW2" t="str">
         <v>yes</v>
       </c>
-      <c r="CQ2" t="str">
+      <c r="DX2" t="str">
         <v>no</v>
       </c>
-      <c r="CR2" t="str">
+      <c r="DY2" t="str">
         <v>yes</v>
       </c>
-      <c r="CS2" t="str">
+      <c r="DZ2" t="str">
         <v>yes</v>
       </c>
-      <c r="CT2" t="str">
+      <c r="EA2" t="str">
         <v>no</v>
       </c>
-      <c r="CU2" t="str">
+      <c r="EB2" t="str">
         <v>yes</v>
       </c>
-      <c r="CV2" t="str">
+      <c r="EC2" t="str">
         <v>yes</v>
       </c>
-      <c r="CW2" t="str">
+      <c r="ED2" t="str">
         <v>Washington University St. Louis, MO</v>
       </c>
-      <c r="CX2">
+      <c r="EE2">
         <v>28976</v>
       </c>
-      <c r="CY2" t="str">
-        <v>-</v>
-      </c>
-      <c r="CZ2" t="str">
-        <v>-</v>
-      </c>
-      <c r="DA2" t="str">
-        <v>-</v>
-      </c>
-      <c r="DB2" t="str">
-        <v>-</v>
-      </c>
-      <c r="DC2" t="str">
-        <v>-</v>
-      </c>
-      <c r="DD2" t="str">
-        <v>-</v>
-      </c>
-      <c r="DE2" t="str">
+      <c r="EF2" t="str">
+        <v>-</v>
+      </c>
+      <c r="EG2" t="str">
+        <v>-</v>
+      </c>
+      <c r="EH2" t="str">
+        <v>-</v>
+      </c>
+      <c r="EI2" t="str">
+        <v>-</v>
+      </c>
+      <c r="EJ2" t="str">
+        <v>-</v>
+      </c>
+      <c r="EK2" t="str">
+        <v>-</v>
+      </c>
+      <c r="EL2" t="str">
         <v>1550 E MARYLAND AVE</v>
       </c>
-      <c r="DF2" t="str">
+      <c r="EM2" t="str">
         <v>Phoenix</v>
       </c>
-      <c r="DG2" t="str">
+      <c r="EN2" t="str">
         <v>AZ</v>
       </c>
-      <c r="DH2">
+      <c r="EO2">
         <v>85014</v>
       </c>
-      <c r="DI2" t="str">
-        <v>-</v>
-      </c>
-      <c r="DJ2" t="str">
-        <v>-</v>
-      </c>
-      <c r="DK2" t="str">
-        <v>-</v>
-      </c>
-      <c r="DL2" t="str">
-        <v>-</v>
-      </c>
-      <c r="DM2" t="str">
-        <v>-</v>
-      </c>
-      <c r="DN2" t="str">
-        <v>-</v>
-      </c>
-      <c r="DO2" t="str">
-        <v>-</v>
-      </c>
-      <c r="DP2" t="str">
-        <v>-</v>
-      </c>
-      <c r="DQ2" t="str">
-        <v>-</v>
-      </c>
-      <c r="DR2" t="str">
-        <v>-</v>
-      </c>
-      <c r="DS2" t="str">
-        <v>-</v>
-      </c>
-      <c r="DT2" t="str">
-        <v>-</v>
-      </c>
-      <c r="DU2" t="str">
-        <v>-</v>
-      </c>
-      <c r="DV2" t="str">
-        <v>-</v>
-      </c>
-      <c r="DW2" t="str">
-        <v>-</v>
-      </c>
-      <c r="DX2" t="str">
-        <v>-</v>
-      </c>
-      <c r="DY2">
+      <c r="EP2" t="str">
+        <v>-</v>
+      </c>
+      <c r="EQ2" t="str">
+        <v>-</v>
+      </c>
+      <c r="ER2" t="str">
+        <v>-</v>
+      </c>
+      <c r="ES2" t="str">
+        <v>-</v>
+      </c>
+      <c r="ET2" t="str">
+        <v>-</v>
+      </c>
+      <c r="EU2" t="str">
+        <v>-</v>
+      </c>
+      <c r="EV2" t="str">
+        <v>-</v>
+      </c>
+      <c r="EW2" t="str">
+        <v>-</v>
+      </c>
+      <c r="EX2" t="str">
+        <v>-</v>
+      </c>
+      <c r="EY2" t="str">
+        <v>-</v>
+      </c>
+      <c r="EZ2" t="str">
+        <v>-</v>
+      </c>
+      <c r="FA2" t="str">
+        <v>-</v>
+      </c>
+      <c r="FB2" t="str">
+        <v>-</v>
+      </c>
+      <c r="FC2" t="str">
+        <v>-</v>
+      </c>
+      <c r="FD2" t="str">
+        <v>-</v>
+      </c>
+      <c r="FE2" t="str">
+        <v>-</v>
+      </c>
+      <c r="FF2">
         <v>6022859979</v>
       </c>
-      <c r="DZ2" t="str">
+      <c r="FG2" t="str">
         <v>marc.arak@gmail.com</v>
       </c>
-      <c r="EA2" t="str">
+      <c r="FH2" t="str">
+        <v>-</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Abbey</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Paul</v>
+      </c>
+      <c r="C3" t="str">
+        <v>-</v>
+      </c>
+      <c r="D3" t="str">
+        <v>-</v>
+      </c>
+      <c r="E3" t="str">
+        <v>-</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Dentist</v>
+      </c>
+      <c r="G3">
+        <v>1891768495</v>
+      </c>
+      <c r="H3" t="str">
+        <v>-</v>
+      </c>
+      <c r="I3" t="str">
+        <v>-</v>
+      </c>
+      <c r="J3" t="str">
+        <v>-</v>
+      </c>
+      <c r="K3" t="str">
+        <v>-</v>
+      </c>
+      <c r="L3" t="str">
+        <v>-</v>
+      </c>
+      <c r="M3" t="str">
+        <v>-</v>
+      </c>
+      <c r="N3" t="str">
+        <v>-</v>
+      </c>
+      <c r="O3" t="str">
+        <v>-</v>
+      </c>
+      <c r="P3" t="str">
+        <v>-</v>
+      </c>
+      <c r="Q3" t="str">
+        <v>-</v>
+      </c>
+      <c r="R3" t="str">
+        <v>-</v>
+      </c>
+      <c r="S3" t="str">
+        <v>-</v>
+      </c>
+      <c r="T3" t="str">
+        <v>DEN.00104931</v>
+      </c>
+      <c r="U3" t="str">
+        <v>colorado</v>
+      </c>
+      <c r="V3" t="str">
+        <v>-</v>
+      </c>
+      <c r="W3" t="str">
+        <v>-</v>
+      </c>
+      <c r="X3" t="str">
+        <v>-</v>
+      </c>
+      <c r="Y3" t="str">
+        <v>-</v>
+      </c>
+      <c r="Z3" t="str">
+        <v>-</v>
+      </c>
+      <c r="AA3" t="str">
+        <v>-</v>
+      </c>
+      <c r="AB3" t="str">
+        <v>-</v>
+      </c>
+      <c r="AC3" t="str">
+        <v>-</v>
+      </c>
+      <c r="AD3" t="str">
+        <v>-</v>
+      </c>
+      <c r="AE3" t="str">
+        <v>-</v>
+      </c>
+      <c r="AF3" t="str">
+        <v>-</v>
+      </c>
+      <c r="AG3" t="str">
+        <v>-</v>
+      </c>
+      <c r="AH3" t="str">
+        <v>-</v>
+      </c>
+      <c r="AI3" t="str">
+        <v>-</v>
+      </c>
+      <c r="AJ3" t="str">
+        <v>-</v>
+      </c>
+      <c r="AK3" t="str">
+        <v>-</v>
+      </c>
+      <c r="AL3" t="str">
+        <v>-</v>
+      </c>
+      <c r="AM3" t="str">
+        <v>-</v>
+      </c>
+      <c r="AN3" t="str">
+        <v>-</v>
+      </c>
+      <c r="AO3" t="str">
+        <v>-</v>
+      </c>
+      <c r="AP3" t="str">
+        <v>-</v>
+      </c>
+      <c r="AQ3" t="str">
+        <v>-</v>
+      </c>
+      <c r="AR3" t="str">
+        <v>-</v>
+      </c>
+      <c r="AS3" t="str">
+        <v>-</v>
+      </c>
+      <c r="AT3" t="str">
+        <v>-</v>
+      </c>
+      <c r="AU3" t="str">
+        <v>-</v>
+      </c>
+      <c r="AV3" t="str">
+        <v>-</v>
+      </c>
+      <c r="AW3" t="str">
+        <v>-</v>
+      </c>
+      <c r="AX3" t="str">
+        <v>-</v>
+      </c>
+      <c r="AY3" t="str">
+        <v>-</v>
+      </c>
+      <c r="AZ3" t="str">
+        <v>-</v>
+      </c>
+      <c r="BA3" t="str">
+        <v>-</v>
+      </c>
+      <c r="BB3" t="str">
+        <v>-</v>
+      </c>
+      <c r="BC3" t="str">
+        <v>-</v>
+      </c>
+      <c r="BD3" t="str">
+        <v>-</v>
+      </c>
+      <c r="BE3" t="str">
+        <v>-</v>
+      </c>
+      <c r="BF3" t="str">
+        <v>-</v>
+      </c>
+      <c r="BG3" t="str">
+        <v>-</v>
+      </c>
+      <c r="BH3" t="str">
+        <v>-</v>
+      </c>
+      <c r="BI3" t="str">
+        <v>-</v>
+      </c>
+      <c r="BJ3" t="str">
+        <v>-</v>
+      </c>
+      <c r="BK3" t="str">
+        <v>-</v>
+      </c>
+      <c r="BL3" t="str">
+        <v>-</v>
+      </c>
+      <c r="BM3" t="str">
+        <v>-</v>
+      </c>
+      <c r="BN3" t="str">
+        <v>-</v>
+      </c>
+      <c r="BO3" t="str">
+        <v>-</v>
+      </c>
+      <c r="BP3" t="str">
+        <v>-</v>
+      </c>
+      <c r="BQ3" t="str">
+        <v>-</v>
+      </c>
+      <c r="BR3" t="str">
+        <v>-</v>
+      </c>
+      <c r="BS3" t="str">
+        <v>-</v>
+      </c>
+      <c r="BT3" t="str">
+        <v>-</v>
+      </c>
+      <c r="BU3" t="str">
+        <v>-</v>
+      </c>
+      <c r="BV3" t="str">
+        <v>-</v>
+      </c>
+      <c r="BW3" t="str">
+        <v>-</v>
+      </c>
+      <c r="BX3" t="str">
+        <v>-</v>
+      </c>
+      <c r="BY3" t="str">
+        <v>-</v>
+      </c>
+      <c r="BZ3" t="str">
+        <v>-</v>
+      </c>
+      <c r="CA3" t="str">
+        <v>-</v>
+      </c>
+      <c r="CB3" t="str">
+        <v>-</v>
+      </c>
+      <c r="CC3" t="str">
+        <v>-</v>
+      </c>
+      <c r="CD3" t="str">
+        <v>-</v>
+      </c>
+      <c r="CE3" t="str">
+        <v>-</v>
+      </c>
+      <c r="CF3" t="str">
+        <v>-</v>
+      </c>
+      <c r="CG3" t="str">
+        <v>-</v>
+      </c>
+      <c r="CH3" t="str">
+        <v>-</v>
+      </c>
+      <c r="CI3" t="str">
+        <v>-</v>
+      </c>
+      <c r="CJ3" t="str">
+        <v>-</v>
+      </c>
+      <c r="CK3" t="str">
+        <v>-</v>
+      </c>
+      <c r="CL3" t="str">
+        <v>-</v>
+      </c>
+      <c r="CM3" t="str">
+        <v>-</v>
+      </c>
+      <c r="CN3" t="str">
+        <v>-</v>
+      </c>
+      <c r="CO3" t="str">
+        <v>-</v>
+      </c>
+      <c r="CP3" t="str">
+        <v>-</v>
+      </c>
+      <c r="CQ3" t="str">
+        <v>-</v>
+      </c>
+      <c r="CR3" t="str">
+        <v>-</v>
+      </c>
+      <c r="CS3" t="str">
+        <v>-</v>
+      </c>
+      <c r="CT3" t="str">
+        <v>-</v>
+      </c>
+      <c r="CU3" t="str">
+        <v>-</v>
+      </c>
+      <c r="CV3" t="str">
+        <v>-</v>
+      </c>
+      <c r="CW3" t="str">
+        <v>-</v>
+      </c>
+      <c r="CX3" t="str">
+        <v>-</v>
+      </c>
+      <c r="CY3" t="str">
+        <v>-</v>
+      </c>
+      <c r="CZ3" t="str">
+        <v>-</v>
+      </c>
+      <c r="DA3" t="str">
+        <v>-</v>
+      </c>
+      <c r="DB3" t="str">
+        <v>-</v>
+      </c>
+      <c r="DC3" t="str">
+        <v>-</v>
+      </c>
+      <c r="DD3" t="str">
+        <v>-</v>
+      </c>
+      <c r="DE3" t="str">
+        <v>-</v>
+      </c>
+      <c r="DF3" t="str">
+        <v>-</v>
+      </c>
+      <c r="DG3" t="str">
+        <v>-</v>
+      </c>
+      <c r="DH3" t="str">
+        <v>-</v>
+      </c>
+      <c r="DI3" t="str">
+        <v>-</v>
+      </c>
+      <c r="DJ3" t="str">
+        <v>-</v>
+      </c>
+      <c r="DK3" t="str">
+        <v>-</v>
+      </c>
+      <c r="DL3" t="str">
+        <v>-</v>
+      </c>
+      <c r="DM3" t="str">
+        <v>-</v>
+      </c>
+      <c r="DN3" t="str">
+        <v>-</v>
+      </c>
+      <c r="DO3" t="str">
+        <v>-</v>
+      </c>
+      <c r="DP3" t="str">
+        <v>-</v>
+      </c>
+      <c r="DQ3" t="str">
+        <v>Paul F. Abbey</v>
+      </c>
+      <c r="DR3">
+        <v>44075</v>
+      </c>
+      <c r="DS3" t="str">
+        <v>-</v>
+      </c>
+      <c r="DT3" t="str">
+        <v>no</v>
+      </c>
+      <c r="DU3" t="str">
+        <v>yes</v>
+      </c>
+      <c r="DV3" t="str">
+        <v>yes</v>
+      </c>
+      <c r="DW3" t="str">
+        <v>yes</v>
+      </c>
+      <c r="DX3" t="str">
+        <v>no</v>
+      </c>
+      <c r="DY3" t="str">
+        <v>yes</v>
+      </c>
+      <c r="DZ3" t="str">
+        <v>yes</v>
+      </c>
+      <c r="EA3" t="str">
+        <v>yes</v>
+      </c>
+      <c r="EB3" t="str">
+        <v>yes</v>
+      </c>
+      <c r="EC3" t="str">
+        <v>yes</v>
+      </c>
+      <c r="ED3" t="str">
+        <v>-</v>
+      </c>
+      <c r="EE3" t="str">
+        <v>-</v>
+      </c>
+      <c r="EF3" t="str">
+        <v>-</v>
+      </c>
+      <c r="EG3" t="str">
+        <v>-</v>
+      </c>
+      <c r="EH3" t="str">
+        <v>-</v>
+      </c>
+      <c r="EI3" t="str">
+        <v>-</v>
+      </c>
+      <c r="EJ3" t="str">
+        <v>-</v>
+      </c>
+      <c r="EK3" t="str">
+        <v>-</v>
+      </c>
+      <c r="EL3" t="str">
+        <v>1507 W MOUNTAIN VIEW AVE</v>
+      </c>
+      <c r="EM3" t="str">
+        <v>LONGMONT</v>
+      </c>
+      <c r="EN3" t="str">
+        <v>CO</v>
+      </c>
+      <c r="EO3" t="str">
+        <v>80501-3201</v>
+      </c>
+      <c r="EP3" t="str">
+        <v>-</v>
+      </c>
+      <c r="EQ3" t="str">
+        <v>-</v>
+      </c>
+      <c r="ER3" t="str">
+        <v>-</v>
+      </c>
+      <c r="ES3" t="str">
+        <v>-</v>
+      </c>
+      <c r="ET3" t="str">
+        <v>-</v>
+      </c>
+      <c r="EU3" t="str">
+        <v>-</v>
+      </c>
+      <c r="EV3" t="str">
+        <v>-</v>
+      </c>
+      <c r="EW3" t="str">
+        <v>-</v>
+      </c>
+      <c r="EX3" t="str">
+        <v>-</v>
+      </c>
+      <c r="EY3" t="str">
+        <v>-</v>
+      </c>
+      <c r="EZ3" t="str">
+        <v>-</v>
+      </c>
+      <c r="FA3" t="str">
+        <v>-</v>
+      </c>
+      <c r="FB3" t="str">
+        <v>-</v>
+      </c>
+      <c r="FC3" t="str">
+        <v>-</v>
+      </c>
+      <c r="FD3" t="str">
+        <v>-</v>
+      </c>
+      <c r="FE3" t="str">
+        <v>-</v>
+      </c>
+      <c r="FF3" t="str">
+        <v>(303) 678-0997</v>
+      </c>
+      <c r="FG3" t="str">
+        <v>paul.abbey@gmail.com</v>
+      </c>
+      <c r="FH3" t="str">
+        <v>-</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Abate</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Martin</v>
+      </c>
+      <c r="C4" t="str">
+        <v>-</v>
+      </c>
+      <c r="D4" t="str">
+        <v>-</v>
+      </c>
+      <c r="E4" t="str">
+        <v>-</v>
+      </c>
+      <c r="F4" t="str">
+        <v>Dentist</v>
+      </c>
+      <c r="G4">
+        <v>1932302106</v>
+      </c>
+      <c r="H4" t="str">
+        <v>-</v>
+      </c>
+      <c r="I4" t="str">
+        <v>-</v>
+      </c>
+      <c r="J4" t="str">
+        <v>-</v>
+      </c>
+      <c r="K4" t="str">
+        <v>-</v>
+      </c>
+      <c r="L4" t="str">
+        <v>-</v>
+      </c>
+      <c r="M4" t="str">
+        <v>-</v>
+      </c>
+      <c r="N4" t="str">
+        <v>-</v>
+      </c>
+      <c r="O4" t="str">
+        <v>-</v>
+      </c>
+      <c r="P4" t="str">
+        <v>-</v>
+      </c>
+      <c r="Q4" t="str">
+        <v>-</v>
+      </c>
+      <c r="R4" t="str">
+        <v>-</v>
+      </c>
+      <c r="S4" t="str">
+        <v>-</v>
+      </c>
+      <c r="T4">
+        <v>37767</v>
+      </c>
+      <c r="U4" t="str">
+        <v>california</v>
+      </c>
+      <c r="V4" t="str">
+        <v>-</v>
+      </c>
+      <c r="W4" t="str">
+        <v>-</v>
+      </c>
+      <c r="X4" t="str">
+        <v>-</v>
+      </c>
+      <c r="Y4" t="str">
+        <v>-</v>
+      </c>
+      <c r="Z4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AA4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AB4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AC4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AD4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AE4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AF4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AG4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AH4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AI4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AJ4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AK4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AL4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AM4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AN4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AO4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AP4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AQ4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AR4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AS4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AT4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AU4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AV4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AW4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AX4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AY4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AZ4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BA4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BB4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BC4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BD4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BE4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BF4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BG4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BH4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BI4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BJ4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BK4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BL4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BM4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BN4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BO4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BP4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BQ4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BR4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BS4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BT4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BU4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BV4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BW4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BX4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BY4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BZ4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CA4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CB4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CC4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CD4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CE4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CF4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CG4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CH4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CI4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CJ4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CK4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CL4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CM4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CN4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CO4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CP4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CQ4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CR4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CS4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CT4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CU4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CV4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CW4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CX4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CY4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CZ4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DA4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DB4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DC4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DD4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DE4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DF4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DG4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DH4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DI4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DJ4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DK4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DL4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DM4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DN4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DO4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DP4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DQ4" t="str">
+        <v>Martin S. Abate</v>
+      </c>
+      <c r="DR4">
+        <v>43835</v>
+      </c>
+      <c r="DS4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DT4" t="str">
+        <v>yes</v>
+      </c>
+      <c r="DU4" t="str">
+        <v>yes</v>
+      </c>
+      <c r="DV4" t="str">
+        <v>no</v>
+      </c>
+      <c r="DW4" t="str">
+        <v>yes</v>
+      </c>
+      <c r="DX4" t="str">
+        <v>yes</v>
+      </c>
+      <c r="DY4" t="str">
+        <v>yes</v>
+      </c>
+      <c r="DZ4" t="str">
+        <v>yes</v>
+      </c>
+      <c r="EA4" t="str">
+        <v>yes</v>
+      </c>
+      <c r="EB4" t="str">
+        <v>yes</v>
+      </c>
+      <c r="EC4" t="str">
+        <v>yes</v>
+      </c>
+      <c r="ED4" t="str">
+        <v>-</v>
+      </c>
+      <c r="EE4" t="str">
+        <v>-</v>
+      </c>
+      <c r="EF4" t="str">
+        <v>-</v>
+      </c>
+      <c r="EG4" t="str">
+        <v>-</v>
+      </c>
+      <c r="EH4" t="str">
+        <v>-</v>
+      </c>
+      <c r="EI4" t="str">
+        <v>-</v>
+      </c>
+      <c r="EJ4" t="str">
+        <v>-</v>
+      </c>
+      <c r="EK4" t="str">
+        <v>-</v>
+      </c>
+      <c r="EL4" t="str">
+        <v>3637 SACRAMENTO ST</v>
+      </c>
+      <c r="EM4" t="str">
+        <v>SAN FRANCISCO</v>
+      </c>
+      <c r="EN4" t="str">
+        <v>CA</v>
+      </c>
+      <c r="EO4">
+        <v>94118</v>
+      </c>
+      <c r="EP4" t="str">
+        <v>-</v>
+      </c>
+      <c r="EQ4" t="str">
+        <v>-</v>
+      </c>
+      <c r="ER4" t="str">
+        <v>-</v>
+      </c>
+      <c r="ES4" t="str">
+        <v>-</v>
+      </c>
+      <c r="ET4" t="str">
+        <v>-</v>
+      </c>
+      <c r="EU4" t="str">
+        <v>-</v>
+      </c>
+      <c r="EV4" t="str">
+        <v>-</v>
+      </c>
+      <c r="EW4" t="str">
+        <v>-</v>
+      </c>
+      <c r="EX4" t="str">
+        <v>-</v>
+      </c>
+      <c r="EY4" t="str">
+        <v>-</v>
+      </c>
+      <c r="EZ4" t="str">
+        <v>-</v>
+      </c>
+      <c r="FA4" t="str">
+        <v>-</v>
+      </c>
+      <c r="FB4" t="str">
+        <v>-</v>
+      </c>
+      <c r="FC4" t="str">
+        <v>-</v>
+      </c>
+      <c r="FD4" t="str">
+        <v>-</v>
+      </c>
+      <c r="FE4" t="str">
+        <v>-</v>
+      </c>
+      <c r="FF4" t="str">
+        <v>415-989-1001</v>
+      </c>
+      <c r="FG4" t="str">
+        <v>martin.abate@gmail.com</v>
+      </c>
+      <c r="FH4" t="str">
+        <v>-</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Yanich</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Jason</v>
+      </c>
+      <c r="C5" t="str">
+        <v>-</v>
+      </c>
+      <c r="D5" t="str">
+        <v>-</v>
+      </c>
+      <c r="E5" t="str">
+        <v>-</v>
+      </c>
+      <c r="F5" t="str">
+        <v>Dentist</v>
+      </c>
+      <c r="G5">
+        <v>1114141793</v>
+      </c>
+      <c r="H5" t="str">
+        <v>-</v>
+      </c>
+      <c r="I5" t="str">
+        <v>-</v>
+      </c>
+      <c r="J5" t="str">
+        <v>-</v>
+      </c>
+      <c r="K5" t="str">
+        <v>-</v>
+      </c>
+      <c r="L5" t="str">
+        <v>-</v>
+      </c>
+      <c r="M5" t="str">
+        <v>-</v>
+      </c>
+      <c r="N5" t="str">
+        <v>-</v>
+      </c>
+      <c r="O5" t="str">
+        <v>-</v>
+      </c>
+      <c r="P5" t="str">
+        <v>-</v>
+      </c>
+      <c r="Q5" t="str">
+        <v>-</v>
+      </c>
+      <c r="R5" t="str">
+        <v>-</v>
+      </c>
+      <c r="S5" t="str">
+        <v>-</v>
+      </c>
+      <c r="T5">
+        <v>30.021662</v>
+      </c>
+      <c r="U5" t="str">
+        <v>ohio</v>
+      </c>
+      <c r="V5" t="str">
+        <v>-</v>
+      </c>
+      <c r="W5" t="str">
+        <v>-</v>
+      </c>
+      <c r="X5" t="str">
+        <v>-</v>
+      </c>
+      <c r="Y5" t="str">
+        <v>-</v>
+      </c>
+      <c r="Z5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AA5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AB5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AC5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AD5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AE5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AF5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AG5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AH5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AI5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AJ5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AK5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AL5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AM5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AN5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AO5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AP5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AQ5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AR5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AS5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AT5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AU5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AV5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AW5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AX5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AY5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AZ5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BA5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BB5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BC5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BD5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BE5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BF5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BG5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BH5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BI5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BJ5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BK5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BL5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BM5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BN5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BO5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BP5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BQ5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BR5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BS5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BT5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BU5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BV5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BW5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BX5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BY5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BZ5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CA5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CB5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CC5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CD5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CE5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CF5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CG5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CH5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CI5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CJ5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CK5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CL5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CM5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CN5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CO5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CP5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CQ5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CR5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CS5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CT5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CU5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CV5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CW5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CX5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CY5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CZ5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DA5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DB5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DC5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DD5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DE5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DF5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DG5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DH5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DI5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DJ5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DK5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DL5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DM5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DN5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DO5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DP5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DQ5" t="str">
+        <v>Jason P. Yanich</v>
+      </c>
+      <c r="DR5">
+        <v>43863</v>
+      </c>
+      <c r="DS5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DT5" t="str">
+        <v>no</v>
+      </c>
+      <c r="DU5" t="str">
+        <v>yes</v>
+      </c>
+      <c r="DV5" t="str">
+        <v>no</v>
+      </c>
+      <c r="DW5" t="str">
+        <v>no</v>
+      </c>
+      <c r="DX5" t="str">
+        <v>no</v>
+      </c>
+      <c r="DY5" t="str">
+        <v>yes</v>
+      </c>
+      <c r="DZ5" t="str">
+        <v>yes</v>
+      </c>
+      <c r="EA5" t="str">
+        <v>yes</v>
+      </c>
+      <c r="EB5" t="str">
+        <v>yes</v>
+      </c>
+      <c r="EC5" t="str">
+        <v>yes</v>
+      </c>
+      <c r="ED5" t="str">
+        <v>-</v>
+      </c>
+      <c r="EE5" t="str">
+        <v>-</v>
+      </c>
+      <c r="EF5" t="str">
+        <v>-</v>
+      </c>
+      <c r="EG5" t="str">
+        <v>-</v>
+      </c>
+      <c r="EH5" t="str">
+        <v>-</v>
+      </c>
+      <c r="EI5" t="str">
+        <v>-</v>
+      </c>
+      <c r="EJ5" t="str">
+        <v>-</v>
+      </c>
+      <c r="EK5" t="str">
+        <v>-</v>
+      </c>
+      <c r="EL5" t="str">
+        <v>1456 MARION WALDO RD</v>
+      </c>
+      <c r="EM5" t="str">
+        <v>MARION</v>
+      </c>
+      <c r="EN5" t="str">
+        <v>OH</v>
+      </c>
+      <c r="EO5" t="str">
+        <v>43302-7422</v>
+      </c>
+      <c r="EP5" t="str">
+        <v>-</v>
+      </c>
+      <c r="EQ5" t="str">
+        <v>-</v>
+      </c>
+      <c r="ER5" t="str">
+        <v>-</v>
+      </c>
+      <c r="ES5" t="str">
+        <v>-</v>
+      </c>
+      <c r="ET5" t="str">
+        <v>-</v>
+      </c>
+      <c r="EU5" t="str">
+        <v>-</v>
+      </c>
+      <c r="EV5" t="str">
+        <v>-</v>
+      </c>
+      <c r="EW5" t="str">
+        <v>-</v>
+      </c>
+      <c r="EX5" t="str">
+        <v>-</v>
+      </c>
+      <c r="EY5" t="str">
+        <v>-</v>
+      </c>
+      <c r="EZ5" t="str">
+        <v>-</v>
+      </c>
+      <c r="FA5" t="str">
+        <v>-</v>
+      </c>
+      <c r="FB5" t="str">
+        <v>-</v>
+      </c>
+      <c r="FC5" t="str">
+        <v>-</v>
+      </c>
+      <c r="FD5" t="str">
+        <v>-</v>
+      </c>
+      <c r="FE5" t="str">
+        <v>-</v>
+      </c>
+      <c r="FF5" t="str">
+        <v>740-389-2100</v>
+      </c>
+      <c r="FG5" t="str">
+        <v>jason.yanich@gmail.com</v>
+      </c>
+      <c r="FH5" t="str">
+        <v>-</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>-</v>
+      </c>
+      <c r="B6" t="str">
+        <v>-</v>
+      </c>
+      <c r="C6" t="str">
+        <v>-</v>
+      </c>
+      <c r="D6" t="str">
+        <v>-</v>
+      </c>
+      <c r="E6" t="str">
+        <v>-</v>
+      </c>
+      <c r="F6" t="str">
+        <v>-</v>
+      </c>
+      <c r="G6" t="str">
+        <v>-</v>
+      </c>
+      <c r="H6" t="str">
+        <v>-</v>
+      </c>
+      <c r="I6" t="str">
+        <v>-</v>
+      </c>
+      <c r="J6" t="str">
+        <v>-</v>
+      </c>
+      <c r="K6" t="str">
+        <v>-</v>
+      </c>
+      <c r="L6" t="str">
+        <v>-</v>
+      </c>
+      <c r="M6" t="str">
+        <v>-</v>
+      </c>
+      <c r="N6" t="str">
+        <v>-</v>
+      </c>
+      <c r="O6" t="str">
+        <v>-</v>
+      </c>
+      <c r="P6" t="str">
+        <v>-</v>
+      </c>
+      <c r="Q6" t="str">
+        <v>-</v>
+      </c>
+      <c r="R6" t="str">
+        <v>-</v>
+      </c>
+      <c r="S6" t="str">
+        <v>-</v>
+      </c>
+      <c r="T6" t="str">
+        <v>-</v>
+      </c>
+      <c r="U6" t="str">
+        <v>-</v>
+      </c>
+      <c r="V6" t="str">
+        <v>-</v>
+      </c>
+      <c r="W6" t="str">
+        <v>-</v>
+      </c>
+      <c r="X6" t="str">
+        <v>-</v>
+      </c>
+      <c r="Y6" t="str">
+        <v>-</v>
+      </c>
+      <c r="Z6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AA6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AB6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AC6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AD6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AE6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AF6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AG6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AH6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AI6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AJ6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AK6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AL6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AM6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AN6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AO6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AP6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AQ6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AR6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AS6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AT6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AU6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AV6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AW6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AX6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AY6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AZ6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BA6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BB6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BC6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BD6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BE6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BF6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BG6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BH6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BI6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BJ6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BK6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BL6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BM6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BN6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BO6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BP6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BQ6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BR6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BS6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BT6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BU6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BV6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BW6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BX6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BY6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BZ6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CA6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CB6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CC6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CD6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CE6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CF6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CG6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CH6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CI6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CJ6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CK6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CL6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CM6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CN6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CO6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CP6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CQ6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CR6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CS6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CT6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CU6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CV6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CW6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CX6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CY6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CZ6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DA6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DB6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DC6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DD6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DE6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DF6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DG6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DH6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DI6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DJ6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DK6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DL6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DM6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DN6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DO6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DP6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DQ6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DR6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DS6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DT6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DU6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DV6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DW6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DX6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DY6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DZ6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EA6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EB6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EC6" t="str">
+        <v>-</v>
+      </c>
+      <c r="ED6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EE6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EF6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EG6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EH6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EI6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EJ6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EK6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EL6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EM6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EN6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EO6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EP6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EQ6" t="str">
+        <v>-</v>
+      </c>
+      <c r="ER6" t="str">
+        <v>-</v>
+      </c>
+      <c r="ES6" t="str">
+        <v>-</v>
+      </c>
+      <c r="ET6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EU6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EV6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EW6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EX6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EY6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EZ6" t="str">
+        <v>-</v>
+      </c>
+      <c r="FA6" t="str">
+        <v>-</v>
+      </c>
+      <c r="FB6" t="str">
+        <v>-</v>
+      </c>
+      <c r="FC6" t="str">
+        <v>-</v>
+      </c>
+      <c r="FD6" t="str">
+        <v>-</v>
+      </c>
+      <c r="FE6" t="str">
+        <v>-</v>
+      </c>
+      <c r="FF6" t="str">
+        <v>-</v>
+      </c>
+      <c r="FG6" t="str">
+        <v>-</v>
+      </c>
+      <c r="FH6" t="str">
         <v>-</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:EA2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:FH6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
button and other stuff
</commit_message>
<xml_diff>
--- a/uploads/output.xlsx
+++ b/uploads/output.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:FI3"/>
+  <dimension ref="A1:FI5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -879,19 +879,19 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>2032175671</v>
+        <v>1032170367</v>
       </c>
       <c r="B2" t="str">
-        <v>Yanich</v>
+        <v>Abbey</v>
       </c>
       <c r="C2" t="str">
-        <v>Jason</v>
+        <v>Paul</v>
       </c>
       <c r="D2" t="str">
         <v>-</v>
       </c>
-      <c r="E2">
-        <v>32916</v>
+      <c r="E2" t="str">
+        <v>-</v>
       </c>
       <c r="F2" t="str">
         <v>-</v>
@@ -900,7 +900,7 @@
         <v>Dentist</v>
       </c>
       <c r="H2">
-        <v>1114141793</v>
+        <v>1891768495</v>
       </c>
       <c r="I2" t="str">
         <v>-</v>
@@ -938,23 +938,23 @@
       <c r="T2" t="str">
         <v>-</v>
       </c>
-      <c r="U2">
-        <v>30.021662</v>
+      <c r="U2" t="str">
+        <v>DEN.00104931</v>
       </c>
       <c r="V2" t="str">
-        <v>ohio</v>
+        <v>colorado</v>
       </c>
       <c r="W2" t="str">
-        <v>JASON P  YANICH</v>
+        <v>Paul Frederick Abbey</v>
       </c>
       <c r="X2" t="str">
-        <v>31-11-2021</v>
+        <v>Active</v>
       </c>
       <c r="Y2" t="str">
-        <v>Active</v>
+        <v>02/28/2022</v>
       </c>
       <c r="Z2" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="AA2" t="str">
         <v>07/08/2020</v>
@@ -1242,10 +1242,10 @@
         <v>-</v>
       </c>
       <c r="DR2" t="str">
-        <v>Jason P. Yanich</v>
+        <v>Paul F. Abbey</v>
       </c>
       <c r="DS2">
-        <v>43863</v>
+        <v>44075</v>
       </c>
       <c r="DT2" t="str">
         <v>-</v>
@@ -1257,10 +1257,10 @@
         <v>yes</v>
       </c>
       <c r="DW2" t="str">
-        <v>no</v>
+        <v>yes</v>
       </c>
       <c r="DX2" t="str">
-        <v>no</v>
+        <v>yes</v>
       </c>
       <c r="DY2" t="str">
         <v>no</v>
@@ -1305,16 +1305,16 @@
         <v>-</v>
       </c>
       <c r="EM2" t="str">
-        <v>1456 MARION WALDO RD</v>
+        <v>1507 W MOUNTAIN VIEW AVE</v>
       </c>
       <c r="EN2" t="str">
-        <v>MARION</v>
+        <v>LONGMONT</v>
       </c>
       <c r="EO2" t="str">
-        <v>OH</v>
+        <v>CO</v>
       </c>
       <c r="EP2" t="str">
-        <v>43302-7422</v>
+        <v>80501-3201</v>
       </c>
       <c r="EQ2" t="str">
         <v>-</v>
@@ -1365,10 +1365,10 @@
         <v>-</v>
       </c>
       <c r="FG2" t="str">
-        <v>740-389-2100</v>
+        <v>(303) 678-0997</v>
       </c>
       <c r="FH2" t="str">
-        <v>jason.yanich@gmail.com</v>
+        <v>paul.abbey@gmail.com</v>
       </c>
       <c r="FI2" t="str">
         <v>-</v>
@@ -1376,19 +1376,19 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>1037036721</v>
+        <v>3432170234</v>
       </c>
       <c r="B3" t="str">
-        <v>KYTEAS</v>
+        <v>Abrams</v>
       </c>
       <c r="C3" t="str">
-        <v>PANAGIOTIS</v>
+        <v>Edward</v>
       </c>
       <c r="D3" t="str">
         <v>-</v>
       </c>
       <c r="E3">
-        <v>34316</v>
+        <v>34350</v>
       </c>
       <c r="F3" t="str">
         <v>-</v>
@@ -1397,7 +1397,7 @@
         <v>Dentist</v>
       </c>
       <c r="H3">
-        <v>1336619469</v>
+        <v>1568575868</v>
       </c>
       <c r="I3" t="str">
         <v>-</v>
@@ -1435,17 +1435,17 @@
       <c r="T3" t="str">
         <v>-</v>
       </c>
-      <c r="U3">
-        <v>863927</v>
+      <c r="U3" t="str">
+        <v>DS025857L</v>
       </c>
       <c r="V3" t="str">
-        <v>texas</v>
+        <v>pennstate</v>
       </c>
       <c r="W3" t="str">
-        <v>PANAGIOTIS  KYTEAS</v>
+        <v>EDWARDABRAMS</v>
       </c>
       <c r="X3" t="str">
-        <v>05/31/2022</v>
+        <v>3/31/2021</v>
       </c>
       <c r="Y3" t="str">
         <v>Active</v>
@@ -1739,25 +1739,25 @@
         <v>-</v>
       </c>
       <c r="DR3" t="str">
-        <v>Kyteas Panagiotis</v>
+        <v>Edward S. Abrams</v>
       </c>
       <c r="DS3">
-        <v>43893</v>
+        <v>43986</v>
       </c>
       <c r="DT3" t="str">
         <v>-</v>
       </c>
       <c r="DU3" t="str">
-        <v>no</v>
+        <v>yes</v>
       </c>
       <c r="DV3" t="str">
         <v>yes</v>
       </c>
       <c r="DW3" t="str">
-        <v>no</v>
+        <v>yes</v>
       </c>
       <c r="DX3" t="str">
-        <v>no</v>
+        <v>yes</v>
       </c>
       <c r="DY3" t="str">
         <v>yes</v>
@@ -1766,114 +1766,1108 @@
         <v>no</v>
       </c>
       <c r="EA3" t="str">
+        <v>no</v>
+      </c>
+      <c r="EB3" t="str">
+        <v>no</v>
+      </c>
+      <c r="EC3" t="str">
+        <v>no</v>
+      </c>
+      <c r="ED3" t="str">
+        <v>no</v>
+      </c>
+      <c r="EE3" t="str">
+        <v>-</v>
+      </c>
+      <c r="EF3" t="str">
+        <v>-</v>
+      </c>
+      <c r="EG3" t="str">
+        <v>-</v>
+      </c>
+      <c r="EH3" t="str">
+        <v>-</v>
+      </c>
+      <c r="EI3" t="str">
+        <v>-</v>
+      </c>
+      <c r="EJ3" t="str">
+        <v>-</v>
+      </c>
+      <c r="EK3" t="str">
+        <v>-</v>
+      </c>
+      <c r="EL3" t="str">
+        <v>-</v>
+      </c>
+      <c r="EM3" t="str">
+        <v>2137 WELSH ROAD, STE 3A</v>
+      </c>
+      <c r="EN3" t="str">
+        <v>PHILADELPHIA</v>
+      </c>
+      <c r="EO3" t="str">
+        <v>PA</v>
+      </c>
+      <c r="EP3">
+        <v>19115</v>
+      </c>
+      <c r="EQ3" t="str">
+        <v>-</v>
+      </c>
+      <c r="ER3" t="str">
+        <v>-</v>
+      </c>
+      <c r="ES3" t="str">
+        <v>-</v>
+      </c>
+      <c r="ET3" t="str">
+        <v>-</v>
+      </c>
+      <c r="EU3" t="str">
+        <v>-</v>
+      </c>
+      <c r="EV3" t="str">
+        <v>-</v>
+      </c>
+      <c r="EW3" t="str">
+        <v>-</v>
+      </c>
+      <c r="EX3" t="str">
+        <v>-</v>
+      </c>
+      <c r="EY3" t="str">
+        <v>-</v>
+      </c>
+      <c r="EZ3" t="str">
+        <v>-</v>
+      </c>
+      <c r="FA3" t="str">
+        <v>-</v>
+      </c>
+      <c r="FB3" t="str">
+        <v>-</v>
+      </c>
+      <c r="FC3" t="str">
+        <v>-</v>
+      </c>
+      <c r="FD3" t="str">
+        <v>-</v>
+      </c>
+      <c r="FE3" t="str">
+        <v>-</v>
+      </c>
+      <c r="FF3" t="str">
+        <v>-</v>
+      </c>
+      <c r="FG3" t="str">
+        <v>215-969-1222</v>
+      </c>
+      <c r="FH3" t="str">
+        <v>abrams.edward@gmail.com</v>
+      </c>
+      <c r="FI3" t="str">
+        <v>-</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>2032175671</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Yanich</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Jason</v>
+      </c>
+      <c r="D4" t="str">
+        <v>-</v>
+      </c>
+      <c r="E4">
+        <v>32916</v>
+      </c>
+      <c r="F4" t="str">
+        <v>-</v>
+      </c>
+      <c r="G4" t="str">
+        <v>Dentist</v>
+      </c>
+      <c r="H4">
+        <v>1114141793</v>
+      </c>
+      <c r="I4" t="str">
+        <v>-</v>
+      </c>
+      <c r="J4" t="str">
+        <v>-</v>
+      </c>
+      <c r="K4" t="str">
+        <v>-</v>
+      </c>
+      <c r="L4" t="str">
+        <v>-</v>
+      </c>
+      <c r="M4" t="str">
+        <v>-</v>
+      </c>
+      <c r="N4" t="str">
+        <v>-</v>
+      </c>
+      <c r="O4" t="str">
+        <v>-</v>
+      </c>
+      <c r="P4" t="str">
+        <v>-</v>
+      </c>
+      <c r="Q4" t="str">
+        <v>-</v>
+      </c>
+      <c r="R4" t="str">
+        <v>-</v>
+      </c>
+      <c r="S4" t="str">
+        <v>-</v>
+      </c>
+      <c r="T4" t="str">
+        <v>-</v>
+      </c>
+      <c r="U4">
+        <v>30.021662</v>
+      </c>
+      <c r="V4" t="str">
+        <v>ohio</v>
+      </c>
+      <c r="W4" t="str">
+        <v>JASON P  YANICH</v>
+      </c>
+      <c r="X4" t="str">
+        <v>31-11-2021</v>
+      </c>
+      <c r="Y4" t="str">
+        <v>Active</v>
+      </c>
+      <c r="Z4" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="AA4" t="str">
+        <v>07/08/2020</v>
+      </c>
+      <c r="AB4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AC4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AD4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AE4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AF4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AG4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AH4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AI4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AJ4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AK4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AL4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AM4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AN4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AO4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AP4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AQ4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AR4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AS4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AT4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AU4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AV4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AW4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AX4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AY4" t="str">
+        <v>-</v>
+      </c>
+      <c r="AZ4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BA4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BB4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BC4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BD4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BE4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BF4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BG4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BH4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BI4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BJ4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BK4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BL4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BM4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BN4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BO4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BP4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BQ4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BR4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BS4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BT4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BU4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BV4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BW4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BX4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BY4" t="str">
+        <v>-</v>
+      </c>
+      <c r="BZ4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CA4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CB4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CC4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CD4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CE4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CF4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CG4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CH4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CI4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CJ4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CK4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CL4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CM4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CN4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CO4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CP4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CQ4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CR4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CS4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CT4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CU4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CV4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CW4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CX4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CY4" t="str">
+        <v>-</v>
+      </c>
+      <c r="CZ4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DA4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DB4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DC4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DD4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DE4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DF4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DG4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DH4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DI4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DJ4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DK4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DL4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DM4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DN4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DO4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DP4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DQ4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DR4" t="str">
+        <v>Jason P. Yanich</v>
+      </c>
+      <c r="DS4">
+        <v>43863</v>
+      </c>
+      <c r="DT4" t="str">
+        <v>-</v>
+      </c>
+      <c r="DU4" t="str">
+        <v>no</v>
+      </c>
+      <c r="DV4" t="str">
         <v>yes</v>
       </c>
-      <c r="EB3" t="str">
+      <c r="DW4" t="str">
+        <v>no</v>
+      </c>
+      <c r="DX4" t="str">
+        <v>no</v>
+      </c>
+      <c r="DY4" t="str">
+        <v>no</v>
+      </c>
+      <c r="DZ4" t="str">
         <v>yes</v>
       </c>
-      <c r="EC3" t="str">
+      <c r="EA4" t="str">
         <v>yes</v>
       </c>
-      <c r="ED3" t="str">
+      <c r="EB4" t="str">
         <v>yes</v>
       </c>
-      <c r="EE3" t="str">
+      <c r="EC4" t="str">
+        <v>yes</v>
+      </c>
+      <c r="ED4" t="str">
+        <v>yes</v>
+      </c>
+      <c r="EE4" t="str">
+        <v>-</v>
+      </c>
+      <c r="EF4" t="str">
+        <v>-</v>
+      </c>
+      <c r="EG4" t="str">
+        <v>-</v>
+      </c>
+      <c r="EH4" t="str">
+        <v>-</v>
+      </c>
+      <c r="EI4" t="str">
+        <v>-</v>
+      </c>
+      <c r="EJ4" t="str">
+        <v>-</v>
+      </c>
+      <c r="EK4" t="str">
+        <v>-</v>
+      </c>
+      <c r="EL4" t="str">
+        <v>-</v>
+      </c>
+      <c r="EM4" t="str">
+        <v>1456 MARION WALDO RD</v>
+      </c>
+      <c r="EN4" t="str">
+        <v>MARION</v>
+      </c>
+      <c r="EO4" t="str">
+        <v>OH</v>
+      </c>
+      <c r="EP4" t="str">
+        <v>43302-7422</v>
+      </c>
+      <c r="EQ4" t="str">
+        <v>-</v>
+      </c>
+      <c r="ER4" t="str">
+        <v>-</v>
+      </c>
+      <c r="ES4" t="str">
+        <v>-</v>
+      </c>
+      <c r="ET4" t="str">
+        <v>-</v>
+      </c>
+      <c r="EU4" t="str">
+        <v>-</v>
+      </c>
+      <c r="EV4" t="str">
+        <v>-</v>
+      </c>
+      <c r="EW4" t="str">
+        <v>-</v>
+      </c>
+      <c r="EX4" t="str">
+        <v>-</v>
+      </c>
+      <c r="EY4" t="str">
+        <v>-</v>
+      </c>
+      <c r="EZ4" t="str">
+        <v>-</v>
+      </c>
+      <c r="FA4" t="str">
+        <v>-</v>
+      </c>
+      <c r="FB4" t="str">
+        <v>-</v>
+      </c>
+      <c r="FC4" t="str">
+        <v>-</v>
+      </c>
+      <c r="FD4" t="str">
+        <v>-</v>
+      </c>
+      <c r="FE4" t="str">
+        <v>-</v>
+      </c>
+      <c r="FF4" t="str">
+        <v>-</v>
+      </c>
+      <c r="FG4" t="str">
+        <v>740-389-2100</v>
+      </c>
+      <c r="FH4" t="str">
+        <v>jason.yanich@gmail.com</v>
+      </c>
+      <c r="FI4" t="str">
+        <v>-</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>1037036721</v>
+      </c>
+      <c r="B5" t="str">
+        <v>KYTEAS</v>
+      </c>
+      <c r="C5" t="str">
+        <v>PANAGIOTIS</v>
+      </c>
+      <c r="D5" t="str">
+        <v>-</v>
+      </c>
+      <c r="E5">
+        <v>34316</v>
+      </c>
+      <c r="F5" t="str">
+        <v>-</v>
+      </c>
+      <c r="G5" t="str">
+        <v>Dentist</v>
+      </c>
+      <c r="H5">
+        <v>1336619469</v>
+      </c>
+      <c r="I5" t="str">
+        <v>-</v>
+      </c>
+      <c r="J5" t="str">
+        <v>-</v>
+      </c>
+      <c r="K5" t="str">
+        <v>-</v>
+      </c>
+      <c r="L5" t="str">
+        <v>-</v>
+      </c>
+      <c r="M5" t="str">
+        <v>-</v>
+      </c>
+      <c r="N5" t="str">
+        <v>-</v>
+      </c>
+      <c r="O5" t="str">
+        <v>-</v>
+      </c>
+      <c r="P5" t="str">
+        <v>-</v>
+      </c>
+      <c r="Q5" t="str">
+        <v>-</v>
+      </c>
+      <c r="R5" t="str">
+        <v>-</v>
+      </c>
+      <c r="S5" t="str">
+        <v>-</v>
+      </c>
+      <c r="T5" t="str">
+        <v>-</v>
+      </c>
+      <c r="U5">
+        <v>863927</v>
+      </c>
+      <c r="V5" t="str">
+        <v>texas</v>
+      </c>
+      <c r="W5" t="str">
+        <v>PANAGIOTIS  KYTEAS</v>
+      </c>
+      <c r="X5" t="str">
+        <v>05/31/2022</v>
+      </c>
+      <c r="Y5" t="str">
+        <v>Active</v>
+      </c>
+      <c r="Z5" t="str">
+        <v>No</v>
+      </c>
+      <c r="AA5" t="str">
+        <v>07/08/2020</v>
+      </c>
+      <c r="AB5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AC5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AD5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AE5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AF5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AG5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AH5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AI5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AJ5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AK5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AL5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AM5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AN5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AO5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AP5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AQ5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AR5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AS5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AT5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AU5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AV5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AW5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AX5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AY5" t="str">
+        <v>-</v>
+      </c>
+      <c r="AZ5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BA5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BB5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BC5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BD5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BE5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BF5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BG5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BH5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BI5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BJ5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BK5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BL5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BM5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BN5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BO5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BP5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BQ5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BR5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BS5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BT5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BU5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BV5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BW5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BX5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BY5" t="str">
+        <v>-</v>
+      </c>
+      <c r="BZ5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CA5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CB5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CC5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CD5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CE5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CF5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CG5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CH5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CI5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CJ5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CK5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CL5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CM5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CN5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CO5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CP5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CQ5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CR5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CS5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CT5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CU5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CV5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CW5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CX5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CY5" t="str">
+        <v>-</v>
+      </c>
+      <c r="CZ5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DA5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DB5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DC5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DD5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DE5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DF5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DG5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DH5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DI5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DJ5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DK5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DL5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DM5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DN5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DO5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DP5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DQ5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DR5" t="str">
+        <v>Kyteas Panagiotis</v>
+      </c>
+      <c r="DS5">
+        <v>43893</v>
+      </c>
+      <c r="DT5" t="str">
+        <v>-</v>
+      </c>
+      <c r="DU5" t="str">
+        <v>no</v>
+      </c>
+      <c r="DV5" t="str">
+        <v>yes</v>
+      </c>
+      <c r="DW5" t="str">
+        <v>no</v>
+      </c>
+      <c r="DX5" t="str">
+        <v>no</v>
+      </c>
+      <c r="DY5" t="str">
+        <v>yes</v>
+      </c>
+      <c r="DZ5" t="str">
+        <v>no</v>
+      </c>
+      <c r="EA5" t="str">
+        <v>yes</v>
+      </c>
+      <c r="EB5" t="str">
+        <v>yes</v>
+      </c>
+      <c r="EC5" t="str">
+        <v>yes</v>
+      </c>
+      <c r="ED5" t="str">
+        <v>yes</v>
+      </c>
+      <c r="EE5" t="str">
         <v>ARISTOTLE UNIVERSITY OF THESSALONIKI</v>
       </c>
-      <c r="EF3">
+      <c r="EF5">
         <v>2012</v>
       </c>
-      <c r="EG3" t="str">
-        <v>-</v>
-      </c>
-      <c r="EH3" t="str">
-        <v>-</v>
-      </c>
-      <c r="EI3" t="str">
-        <v>-</v>
-      </c>
-      <c r="EJ3" t="str">
-        <v>-</v>
-      </c>
-      <c r="EK3" t="str">
-        <v>-</v>
-      </c>
-      <c r="EL3" t="str">
-        <v>-</v>
-      </c>
-      <c r="EM3" t="str">
+      <c r="EG5" t="str">
+        <v>-</v>
+      </c>
+      <c r="EH5" t="str">
+        <v>-</v>
+      </c>
+      <c r="EI5" t="str">
+        <v>-</v>
+      </c>
+      <c r="EJ5" t="str">
+        <v>-</v>
+      </c>
+      <c r="EK5" t="str">
+        <v>-</v>
+      </c>
+      <c r="EL5" t="str">
+        <v>-</v>
+      </c>
+      <c r="EM5" t="str">
         <v>21685 KINGSLAND BLVD</v>
       </c>
-      <c r="EN3" t="str">
+      <c r="EN5" t="str">
         <v>KATY</v>
       </c>
-      <c r="EO3" t="str">
+      <c r="EO5" t="str">
         <v>TX</v>
       </c>
-      <c r="EP3" t="str">
+      <c r="EP5" t="str">
         <v>77450-2512</v>
       </c>
-      <c r="EQ3" t="str">
-        <v>-</v>
-      </c>
-      <c r="ER3" t="str">
-        <v>-</v>
-      </c>
-      <c r="ES3" t="str">
-        <v>-</v>
-      </c>
-      <c r="ET3" t="str">
-        <v>-</v>
-      </c>
-      <c r="EU3" t="str">
-        <v>-</v>
-      </c>
-      <c r="EV3" t="str">
-        <v>-</v>
-      </c>
-      <c r="EW3" t="str">
-        <v>-</v>
-      </c>
-      <c r="EX3" t="str">
-        <v>-</v>
-      </c>
-      <c r="EY3" t="str">
-        <v>-</v>
-      </c>
-      <c r="EZ3" t="str">
-        <v>-</v>
-      </c>
-      <c r="FA3" t="str">
-        <v>-</v>
-      </c>
-      <c r="FB3" t="str">
-        <v>-</v>
-      </c>
-      <c r="FC3" t="str">
-        <v>-</v>
-      </c>
-      <c r="FD3" t="str">
-        <v>-</v>
-      </c>
-      <c r="FE3" t="str">
-        <v>-</v>
-      </c>
-      <c r="FF3" t="str">
-        <v>-</v>
-      </c>
-      <c r="FG3" t="str">
+      <c r="EQ5" t="str">
+        <v>-</v>
+      </c>
+      <c r="ER5" t="str">
+        <v>-</v>
+      </c>
+      <c r="ES5" t="str">
+        <v>-</v>
+      </c>
+      <c r="ET5" t="str">
+        <v>-</v>
+      </c>
+      <c r="EU5" t="str">
+        <v>-</v>
+      </c>
+      <c r="EV5" t="str">
+        <v>-</v>
+      </c>
+      <c r="EW5" t="str">
+        <v>-</v>
+      </c>
+      <c r="EX5" t="str">
+        <v>-</v>
+      </c>
+      <c r="EY5" t="str">
+        <v>-</v>
+      </c>
+      <c r="EZ5" t="str">
+        <v>-</v>
+      </c>
+      <c r="FA5" t="str">
+        <v>-</v>
+      </c>
+      <c r="FB5" t="str">
+        <v>-</v>
+      </c>
+      <c r="FC5" t="str">
+        <v>-</v>
+      </c>
+      <c r="FD5" t="str">
+        <v>-</v>
+      </c>
+      <c r="FE5" t="str">
+        <v>-</v>
+      </c>
+      <c r="FF5" t="str">
+        <v>-</v>
+      </c>
+      <c r="FG5" t="str">
         <v>281-578-0008</v>
       </c>
-      <c r="FH3" t="str">
+      <c r="FH5" t="str">
         <v>kyteas.panagiotis@gmail.com</v>
       </c>
-      <c r="FI3" t="str">
+      <c r="FI5" t="str">
         <v>-</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:FI3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:FI5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
oig and npi added
</commit_message>
<xml_diff>
--- a/uploads/output.xlsx
+++ b/uploads/output.xlsx
@@ -903,7 +903,7 @@
         <v>1891768495</v>
       </c>
       <c r="I2" t="str">
-        <v>-</v>
+        <v>PAUL FREDERICK ABBEY</v>
       </c>
       <c r="J2" t="str">
         <v>-</v>
@@ -927,7 +927,7 @@
         <v>-</v>
       </c>
       <c r="Q2" t="str">
-        <v>-</v>
+        <v>CLEAN</v>
       </c>
       <c r="R2" t="str">
         <v>-</v>
@@ -957,7 +957,7 @@
         <v>No</v>
       </c>
       <c r="AA2" t="str">
-        <v>07/08/2020</v>
+        <v>07/09/2020</v>
       </c>
       <c r="AB2" t="str">
         <v>-</v>
@@ -1400,7 +1400,7 @@
         <v>1568575868</v>
       </c>
       <c r="I3" t="str">
-        <v>-</v>
+        <v>EDWARD SCOTT ABRAMS</v>
       </c>
       <c r="J3" t="str">
         <v>-</v>
@@ -1424,7 +1424,7 @@
         <v>-</v>
       </c>
       <c r="Q3" t="str">
-        <v>-</v>
+        <v>CLEAN</v>
       </c>
       <c r="R3" t="str">
         <v>-</v>
@@ -1454,7 +1454,7 @@
         <v>No</v>
       </c>
       <c r="AA3" t="str">
-        <v>07/08/2020</v>
+        <v>07/09/2020</v>
       </c>
       <c r="AB3" t="str">
         <v>-</v>
@@ -1897,7 +1897,7 @@
         <v>1114141793</v>
       </c>
       <c r="I4" t="str">
-        <v>-</v>
+        <v>JASON P YANICH</v>
       </c>
       <c r="J4" t="str">
         <v>-</v>
@@ -1921,7 +1921,7 @@
         <v>-</v>
       </c>
       <c r="Q4" t="str">
-        <v>-</v>
+        <v>CLEAN</v>
       </c>
       <c r="R4" t="str">
         <v>-</v>
@@ -1951,7 +1951,7 @@
         <v>Yes</v>
       </c>
       <c r="AA4" t="str">
-        <v>07/08/2020</v>
+        <v>07/09/2020</v>
       </c>
       <c r="AB4" t="str">
         <v>-</v>
@@ -2394,7 +2394,7 @@
         <v>1336619469</v>
       </c>
       <c r="I5" t="str">
-        <v>-</v>
+        <v>PANAGIOTIS  KYTEAS</v>
       </c>
       <c r="J5" t="str">
         <v>-</v>
@@ -2418,7 +2418,7 @@
         <v>-</v>
       </c>
       <c r="Q5" t="str">
-        <v>-</v>
+        <v>CLEAN</v>
       </c>
       <c r="R5" t="str">
         <v>-</v>
@@ -2448,7 +2448,7 @@
         <v>No</v>
       </c>
       <c r="AA5" t="str">
-        <v>07/08/2020</v>
+        <v>07/09/2020</v>
       </c>
       <c r="AB5" t="str">
         <v>-</v>

</xml_diff>

<commit_message>
error handled and code for deployment
</commit_message>
<xml_diff>
--- a/uploads/output.xlsx
+++ b/uploads/output.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:FI5"/>
+  <dimension ref="A1:FJ9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -876,6 +876,9 @@
       <c r="FI1" t="str">
         <v>dentist's email for correspondence</v>
       </c>
+      <c r="FJ1" t="str">
+        <v>__EMPTY</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2">
@@ -930,7 +933,7 @@
         <v>CLEAN</v>
       </c>
       <c r="R2" t="str">
-        <v>-</v>
+        <v>07/09/2020</v>
       </c>
       <c r="S2" t="str">
         <v>-</v>
@@ -1427,7 +1430,7 @@
         <v>CLEAN</v>
       </c>
       <c r="R3" t="str">
-        <v>-</v>
+        <v>07/09/2020</v>
       </c>
       <c r="S3" t="str">
         <v>-</v>
@@ -1924,7 +1927,7 @@
         <v>CLEAN</v>
       </c>
       <c r="R4" t="str">
-        <v>-</v>
+        <v>07/09/2020</v>
       </c>
       <c r="S4" t="str">
         <v>-</v>
@@ -2421,7 +2424,7 @@
         <v>CLEAN</v>
       </c>
       <c r="R5" t="str">
-        <v>-</v>
+        <v>07/09/2020</v>
       </c>
       <c r="S5" t="str">
         <v>-</v>
@@ -2863,11 +2866,2011 @@
       </c>
       <c r="FI5" t="str">
         <v>-</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>4567703611</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Arak</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Marc</v>
+      </c>
+      <c r="D6" t="str">
+        <v>-</v>
+      </c>
+      <c r="E6">
+        <v>33985</v>
+      </c>
+      <c r="F6" t="str">
+        <v>-</v>
+      </c>
+      <c r="G6" t="str">
+        <v>Dentist</v>
+      </c>
+      <c r="H6">
+        <v>1790897486</v>
+      </c>
+      <c r="I6" t="str">
+        <v>MARC TODD ARAK</v>
+      </c>
+      <c r="J6" t="str">
+        <v>-</v>
+      </c>
+      <c r="K6" t="str">
+        <v>-</v>
+      </c>
+      <c r="L6" t="str">
+        <v>-</v>
+      </c>
+      <c r="M6" t="str">
+        <v>-</v>
+      </c>
+      <c r="N6" t="str">
+        <v>-</v>
+      </c>
+      <c r="O6" t="str">
+        <v>-</v>
+      </c>
+      <c r="P6" t="str">
+        <v>-</v>
+      </c>
+      <c r="Q6" t="str">
+        <v>CLEAN</v>
+      </c>
+      <c r="R6" t="str">
+        <v>07/09/2020</v>
+      </c>
+      <c r="S6" t="str">
+        <v>-</v>
+      </c>
+      <c r="T6" t="str">
+        <v>-</v>
+      </c>
+      <c r="U6" t="str">
+        <v>D02502</v>
+      </c>
+      <c r="V6" t="str">
+        <v>arizona</v>
+      </c>
+      <c r="W6" t="str">
+        <v>Marc T. Arak  DMD</v>
+      </c>
+      <c r="X6" t="str">
+        <v>12/31/2020</v>
+      </c>
+      <c r="Y6" t="str">
+        <v>Active</v>
+      </c>
+      <c r="Z6" t="str">
+        <v>No</v>
+      </c>
+      <c r="AA6" t="str">
+        <v>07/09/2020</v>
+      </c>
+      <c r="AB6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AC6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AD6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AE6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AF6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AG6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AH6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AI6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AJ6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AK6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AL6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AM6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AN6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AO6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AP6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AQ6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AR6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AS6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AT6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AU6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AV6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AW6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AX6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AY6" t="str">
+        <v>-</v>
+      </c>
+      <c r="AZ6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BA6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BB6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BC6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BD6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BE6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BF6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BG6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BH6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BI6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BJ6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BK6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BL6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BM6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BN6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BO6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BP6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BQ6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BR6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BS6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BT6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BU6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BV6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BW6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BX6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BY6" t="str">
+        <v>-</v>
+      </c>
+      <c r="BZ6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CA6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CB6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CC6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CD6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CE6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CF6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CG6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CH6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CI6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CJ6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CK6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CL6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CM6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CN6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CO6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CP6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CQ6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CR6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CS6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CT6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CU6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CV6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CW6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CX6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CY6" t="str">
+        <v>-</v>
+      </c>
+      <c r="CZ6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DA6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DB6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DC6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DD6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DE6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DF6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DG6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DH6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DI6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DJ6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DK6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DL6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DM6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DN6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DO6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DP6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DQ6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DR6" t="str">
+        <v>Marc T. Arak</v>
+      </c>
+      <c r="DS6">
+        <v>43893</v>
+      </c>
+      <c r="DT6" t="str">
+        <v>-</v>
+      </c>
+      <c r="DU6" t="str">
+        <v>yes</v>
+      </c>
+      <c r="DV6" t="str">
+        <v>no</v>
+      </c>
+      <c r="DW6" t="str">
+        <v>yes</v>
+      </c>
+      <c r="DX6" t="str">
+        <v>yes</v>
+      </c>
+      <c r="DY6" t="str">
+        <v>no</v>
+      </c>
+      <c r="DZ6" t="str">
+        <v>yes</v>
+      </c>
+      <c r="EA6" t="str">
+        <v>yes</v>
+      </c>
+      <c r="EB6" t="str">
+        <v>no</v>
+      </c>
+      <c r="EC6" t="str">
+        <v>yes</v>
+      </c>
+      <c r="ED6" t="str">
+        <v>yes</v>
+      </c>
+      <c r="EE6" t="str">
+        <v>Washington University St. Louis, MO</v>
+      </c>
+      <c r="EF6">
+        <v>28860</v>
+      </c>
+      <c r="EG6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EH6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EI6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EJ6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EK6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EL6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EM6" t="str">
+        <v>1550 E MARYLAND AVE</v>
+      </c>
+      <c r="EN6" t="str">
+        <v>Phoenix</v>
+      </c>
+      <c r="EO6" t="str">
+        <v>AZ</v>
+      </c>
+      <c r="EP6">
+        <v>85014</v>
+      </c>
+      <c r="EQ6" t="str">
+        <v>-</v>
+      </c>
+      <c r="ER6" t="str">
+        <v>-</v>
+      </c>
+      <c r="ES6" t="str">
+        <v>-</v>
+      </c>
+      <c r="ET6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EU6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EV6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EW6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EX6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EY6" t="str">
+        <v>-</v>
+      </c>
+      <c r="EZ6" t="str">
+        <v>-</v>
+      </c>
+      <c r="FA6" t="str">
+        <v>-</v>
+      </c>
+      <c r="FB6" t="str">
+        <v>-</v>
+      </c>
+      <c r="FC6" t="str">
+        <v>-</v>
+      </c>
+      <c r="FD6" t="str">
+        <v>-</v>
+      </c>
+      <c r="FE6" t="str">
+        <v>-</v>
+      </c>
+      <c r="FF6" t="str">
+        <v>-</v>
+      </c>
+      <c r="FG6">
+        <v>6022859979</v>
+      </c>
+      <c r="FH6" t="str">
+        <v>marc.arak@gmail.com</v>
+      </c>
+      <c r="FI6" t="str">
+        <v>-</v>
+      </c>
+      <c r="FJ6" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>4103703647</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Wadkar</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Abhinav</v>
+      </c>
+      <c r="D7" t="str">
+        <v>-</v>
+      </c>
+      <c r="E7">
+        <v>32944</v>
+      </c>
+      <c r="F7" t="str">
+        <v>-</v>
+      </c>
+      <c r="G7" t="str">
+        <v>Dentist</v>
+      </c>
+      <c r="H7">
+        <v>1306289772</v>
+      </c>
+      <c r="I7" t="str">
+        <v>ABHINAV P WADKAR</v>
+      </c>
+      <c r="J7" t="str">
+        <v>-</v>
+      </c>
+      <c r="K7" t="str">
+        <v>-</v>
+      </c>
+      <c r="L7" t="str">
+        <v>-</v>
+      </c>
+      <c r="M7" t="str">
+        <v>-</v>
+      </c>
+      <c r="N7" t="str">
+        <v>-</v>
+      </c>
+      <c r="O7" t="str">
+        <v>-</v>
+      </c>
+      <c r="P7" t="str">
+        <v>-</v>
+      </c>
+      <c r="Q7" t="str">
+        <v>CLEAN</v>
+      </c>
+      <c r="R7" t="str">
+        <v>07/09/2020</v>
+      </c>
+      <c r="S7" t="str">
+        <v>-</v>
+      </c>
+      <c r="T7" t="str">
+        <v>-</v>
+      </c>
+      <c r="U7" t="str">
+        <v>22DI02800900</v>
+      </c>
+      <c r="V7" t="str">
+        <v>newjersey</v>
+      </c>
+      <c r="W7" t="str">
+        <v>Abhinav  Wadkar</v>
+      </c>
+      <c r="X7" t="str">
+        <v>31/10/2021</v>
+      </c>
+      <c r="Y7" t="str">
+        <v>Active</v>
+      </c>
+      <c r="Z7" t="str">
+        <v>No</v>
+      </c>
+      <c r="AA7" t="str">
+        <v>07/09/2020</v>
+      </c>
+      <c r="AB7" t="str">
+        <v>-</v>
+      </c>
+      <c r="AC7" t="str">
+        <v>-</v>
+      </c>
+      <c r="AD7" t="str">
+        <v>-</v>
+      </c>
+      <c r="AE7" t="str">
+        <v>-</v>
+      </c>
+      <c r="AF7" t="str">
+        <v>-</v>
+      </c>
+      <c r="AG7" t="str">
+        <v>-</v>
+      </c>
+      <c r="AH7" t="str">
+        <v>-</v>
+      </c>
+      <c r="AI7" t="str">
+        <v>-</v>
+      </c>
+      <c r="AJ7" t="str">
+        <v>-</v>
+      </c>
+      <c r="AK7" t="str">
+        <v>-</v>
+      </c>
+      <c r="AL7" t="str">
+        <v>-</v>
+      </c>
+      <c r="AM7" t="str">
+        <v>-</v>
+      </c>
+      <c r="AN7" t="str">
+        <v>-</v>
+      </c>
+      <c r="AO7" t="str">
+        <v>-</v>
+      </c>
+      <c r="AP7" t="str">
+        <v>-</v>
+      </c>
+      <c r="AQ7" t="str">
+        <v>-</v>
+      </c>
+      <c r="AR7" t="str">
+        <v>-</v>
+      </c>
+      <c r="AS7" t="str">
+        <v>-</v>
+      </c>
+      <c r="AT7" t="str">
+        <v>-</v>
+      </c>
+      <c r="AU7" t="str">
+        <v>-</v>
+      </c>
+      <c r="AV7" t="str">
+        <v>-</v>
+      </c>
+      <c r="AW7" t="str">
+        <v>-</v>
+      </c>
+      <c r="AX7" t="str">
+        <v>-</v>
+      </c>
+      <c r="AY7" t="str">
+        <v>-</v>
+      </c>
+      <c r="AZ7" t="str">
+        <v>-</v>
+      </c>
+      <c r="BA7" t="str">
+        <v>-</v>
+      </c>
+      <c r="BB7" t="str">
+        <v>-</v>
+      </c>
+      <c r="BC7" t="str">
+        <v>-</v>
+      </c>
+      <c r="BD7" t="str">
+        <v>-</v>
+      </c>
+      <c r="BE7" t="str">
+        <v>-</v>
+      </c>
+      <c r="BF7" t="str">
+        <v>-</v>
+      </c>
+      <c r="BG7" t="str">
+        <v>-</v>
+      </c>
+      <c r="BH7" t="str">
+        <v>-</v>
+      </c>
+      <c r="BI7" t="str">
+        <v>-</v>
+      </c>
+      <c r="BJ7" t="str">
+        <v>-</v>
+      </c>
+      <c r="BK7" t="str">
+        <v>-</v>
+      </c>
+      <c r="BL7" t="str">
+        <v>-</v>
+      </c>
+      <c r="BM7" t="str">
+        <v>-</v>
+      </c>
+      <c r="BN7" t="str">
+        <v>-</v>
+      </c>
+      <c r="BO7" t="str">
+        <v>-</v>
+      </c>
+      <c r="BP7" t="str">
+        <v>-</v>
+      </c>
+      <c r="BQ7" t="str">
+        <v>-</v>
+      </c>
+      <c r="BR7" t="str">
+        <v>-</v>
+      </c>
+      <c r="BS7" t="str">
+        <v>-</v>
+      </c>
+      <c r="BT7" t="str">
+        <v>-</v>
+      </c>
+      <c r="BU7" t="str">
+        <v>-</v>
+      </c>
+      <c r="BV7" t="str">
+        <v>-</v>
+      </c>
+      <c r="BW7" t="str">
+        <v>-</v>
+      </c>
+      <c r="BX7" t="str">
+        <v>-</v>
+      </c>
+      <c r="BY7" t="str">
+        <v>-</v>
+      </c>
+      <c r="BZ7" t="str">
+        <v>-</v>
+      </c>
+      <c r="CA7" t="str">
+        <v>-</v>
+      </c>
+      <c r="CB7" t="str">
+        <v>-</v>
+      </c>
+      <c r="CC7" t="str">
+        <v>-</v>
+      </c>
+      <c r="CD7" t="str">
+        <v>-</v>
+      </c>
+      <c r="CE7" t="str">
+        <v>-</v>
+      </c>
+      <c r="CF7" t="str">
+        <v>-</v>
+      </c>
+      <c r="CG7" t="str">
+        <v>-</v>
+      </c>
+      <c r="CH7" t="str">
+        <v>-</v>
+      </c>
+      <c r="CI7" t="str">
+        <v>-</v>
+      </c>
+      <c r="CJ7" t="str">
+        <v>-</v>
+      </c>
+      <c r="CK7" t="str">
+        <v>-</v>
+      </c>
+      <c r="CL7" t="str">
+        <v>-</v>
+      </c>
+      <c r="CM7" t="str">
+        <v>-</v>
+      </c>
+      <c r="CN7" t="str">
+        <v>-</v>
+      </c>
+      <c r="CO7" t="str">
+        <v>-</v>
+      </c>
+      <c r="CP7" t="str">
+        <v>-</v>
+      </c>
+      <c r="CQ7" t="str">
+        <v>-</v>
+      </c>
+      <c r="CR7" t="str">
+        <v>-</v>
+      </c>
+      <c r="CS7" t="str">
+        <v>-</v>
+      </c>
+      <c r="CT7" t="str">
+        <v>-</v>
+      </c>
+      <c r="CU7" t="str">
+        <v>-</v>
+      </c>
+      <c r="CV7" t="str">
+        <v>-</v>
+      </c>
+      <c r="CW7" t="str">
+        <v>-</v>
+      </c>
+      <c r="CX7" t="str">
+        <v>-</v>
+      </c>
+      <c r="CY7" t="str">
+        <v>-</v>
+      </c>
+      <c r="CZ7" t="str">
+        <v>-</v>
+      </c>
+      <c r="DA7" t="str">
+        <v>-</v>
+      </c>
+      <c r="DB7" t="str">
+        <v>-</v>
+      </c>
+      <c r="DC7" t="str">
+        <v>-</v>
+      </c>
+      <c r="DD7" t="str">
+        <v>-</v>
+      </c>
+      <c r="DE7" t="str">
+        <v>-</v>
+      </c>
+      <c r="DF7" t="str">
+        <v>-</v>
+      </c>
+      <c r="DG7" t="str">
+        <v>-</v>
+      </c>
+      <c r="DH7" t="str">
+        <v>-</v>
+      </c>
+      <c r="DI7" t="str">
+        <v>-</v>
+      </c>
+      <c r="DJ7" t="str">
+        <v>-</v>
+      </c>
+      <c r="DK7" t="str">
+        <v>-</v>
+      </c>
+      <c r="DL7" t="str">
+        <v>-</v>
+      </c>
+      <c r="DM7" t="str">
+        <v>-</v>
+      </c>
+      <c r="DN7" t="str">
+        <v>-</v>
+      </c>
+      <c r="DO7" t="str">
+        <v>-</v>
+      </c>
+      <c r="DP7" t="str">
+        <v>-</v>
+      </c>
+      <c r="DQ7" t="str">
+        <v>-</v>
+      </c>
+      <c r="DR7" t="str">
+        <v>Abhinav Wadkar</v>
+      </c>
+      <c r="DS7">
+        <v>43863</v>
+      </c>
+      <c r="DT7" t="str">
+        <v>-</v>
+      </c>
+      <c r="DU7" t="str">
+        <v>yes</v>
+      </c>
+      <c r="DV7" t="str">
+        <v>no</v>
+      </c>
+      <c r="DW7" t="str">
+        <v>yes</v>
+      </c>
+      <c r="DX7" t="str">
+        <v>yes</v>
+      </c>
+      <c r="DY7" t="str">
+        <v>no</v>
+      </c>
+      <c r="DZ7" t="str">
+        <v>yes</v>
+      </c>
+      <c r="EA7" t="str">
+        <v>no</v>
+      </c>
+      <c r="EB7" t="str">
+        <v>no</v>
+      </c>
+      <c r="EC7" t="str">
+        <v>no</v>
+      </c>
+      <c r="ED7" t="str">
+        <v>no</v>
+      </c>
+      <c r="EE7" t="str">
+        <v>Rutgers School of Dental Medicine</v>
+      </c>
+      <c r="EF7" t="str">
+        <v>-</v>
+      </c>
+      <c r="EG7" t="str">
+        <v>-</v>
+      </c>
+      <c r="EH7" t="str">
+        <v>-</v>
+      </c>
+      <c r="EI7" t="str">
+        <v>-</v>
+      </c>
+      <c r="EJ7" t="str">
+        <v>-</v>
+      </c>
+      <c r="EK7" t="str">
+        <v>-</v>
+      </c>
+      <c r="EL7" t="str">
+        <v>-</v>
+      </c>
+      <c r="EM7" t="str">
+        <v>110 BERGEN ST, ROOM D-830</v>
+      </c>
+      <c r="EN7" t="str">
+        <v>NEWARK</v>
+      </c>
+      <c r="EO7" t="str">
+        <v>NJ</v>
+      </c>
+      <c r="EP7" t="str">
+        <v>07103-2495</v>
+      </c>
+      <c r="EQ7" t="str">
+        <v>-</v>
+      </c>
+      <c r="ER7" t="str">
+        <v>-</v>
+      </c>
+      <c r="ES7" t="str">
+        <v>-</v>
+      </c>
+      <c r="ET7" t="str">
+        <v>-</v>
+      </c>
+      <c r="EU7" t="str">
+        <v>-</v>
+      </c>
+      <c r="EV7" t="str">
+        <v>-</v>
+      </c>
+      <c r="EW7" t="str">
+        <v>-</v>
+      </c>
+      <c r="EX7" t="str">
+        <v>-</v>
+      </c>
+      <c r="EY7" t="str">
+        <v>-</v>
+      </c>
+      <c r="EZ7" t="str">
+        <v>-</v>
+      </c>
+      <c r="FA7" t="str">
+        <v>-</v>
+      </c>
+      <c r="FB7" t="str">
+        <v>-</v>
+      </c>
+      <c r="FC7" t="str">
+        <v>-</v>
+      </c>
+      <c r="FD7" t="str">
+        <v>-</v>
+      </c>
+      <c r="FE7" t="str">
+        <v>-</v>
+      </c>
+      <c r="FF7" t="str">
+        <v>-</v>
+      </c>
+      <c r="FG7" t="str">
+        <v>973-972-4615</v>
+      </c>
+      <c r="FH7" t="str">
+        <v>wadkar.abhinav@gmail.com</v>
+      </c>
+      <c r="FI7" t="str">
+        <v>-</v>
+      </c>
+      <c r="FJ7" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>1237036756</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Gill</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Aaftab</v>
+      </c>
+      <c r="D8" t="str">
+        <v>-</v>
+      </c>
+      <c r="E8">
+        <v>34715</v>
+      </c>
+      <c r="F8" t="str">
+        <v>-</v>
+      </c>
+      <c r="G8" t="str">
+        <v>Dentist</v>
+      </c>
+      <c r="H8">
+        <v>1063793834</v>
+      </c>
+      <c r="I8" t="str">
+        <v>AAFTAB SINGH GILL</v>
+      </c>
+      <c r="J8" t="str">
+        <v>-</v>
+      </c>
+      <c r="K8" t="str">
+        <v>-</v>
+      </c>
+      <c r="L8" t="str">
+        <v>-</v>
+      </c>
+      <c r="M8" t="str">
+        <v>-</v>
+      </c>
+      <c r="N8" t="str">
+        <v>-</v>
+      </c>
+      <c r="O8" t="str">
+        <v>-</v>
+      </c>
+      <c r="P8" t="str">
+        <v>-</v>
+      </c>
+      <c r="Q8" t="str">
+        <v>CLEAN</v>
+      </c>
+      <c r="R8" t="str">
+        <v>07/09/2020</v>
+      </c>
+      <c r="S8" t="str">
+        <v>-</v>
+      </c>
+      <c r="T8" t="str">
+        <v>-</v>
+      </c>
+      <c r="U8" t="str">
+        <v>22DI02589200</v>
+      </c>
+      <c r="V8" t="str">
+        <v>massachusetts</v>
+      </c>
+      <c r="W8" t="str">
+        <v>-</v>
+      </c>
+      <c r="X8" t="str">
+        <v>-</v>
+      </c>
+      <c r="Y8" t="str">
+        <v>-</v>
+      </c>
+      <c r="Z8" t="str">
+        <v>-</v>
+      </c>
+      <c r="AA8" t="str">
+        <v>-</v>
+      </c>
+      <c r="AB8" t="str">
+        <v>-</v>
+      </c>
+      <c r="AC8" t="str">
+        <v>-</v>
+      </c>
+      <c r="AD8" t="str">
+        <v>-</v>
+      </c>
+      <c r="AE8" t="str">
+        <v>-</v>
+      </c>
+      <c r="AF8" t="str">
+        <v>-</v>
+      </c>
+      <c r="AG8" t="str">
+        <v>-</v>
+      </c>
+      <c r="AH8" t="str">
+        <v>-</v>
+      </c>
+      <c r="AI8" t="str">
+        <v>-</v>
+      </c>
+      <c r="AJ8" t="str">
+        <v>-</v>
+      </c>
+      <c r="AK8" t="str">
+        <v>-</v>
+      </c>
+      <c r="AL8" t="str">
+        <v>-</v>
+      </c>
+      <c r="AM8" t="str">
+        <v>-</v>
+      </c>
+      <c r="AN8" t="str">
+        <v>-</v>
+      </c>
+      <c r="AO8" t="str">
+        <v>-</v>
+      </c>
+      <c r="AP8" t="str">
+        <v>-</v>
+      </c>
+      <c r="AQ8" t="str">
+        <v>-</v>
+      </c>
+      <c r="AR8" t="str">
+        <v>-</v>
+      </c>
+      <c r="AS8" t="str">
+        <v>-</v>
+      </c>
+      <c r="AT8" t="str">
+        <v>-</v>
+      </c>
+      <c r="AU8" t="str">
+        <v>-</v>
+      </c>
+      <c r="AV8" t="str">
+        <v>-</v>
+      </c>
+      <c r="AW8" t="str">
+        <v>-</v>
+      </c>
+      <c r="AX8" t="str">
+        <v>-</v>
+      </c>
+      <c r="AY8" t="str">
+        <v>-</v>
+      </c>
+      <c r="AZ8" t="str">
+        <v>-</v>
+      </c>
+      <c r="BA8" t="str">
+        <v>-</v>
+      </c>
+      <c r="BB8" t="str">
+        <v>-</v>
+      </c>
+      <c r="BC8" t="str">
+        <v>-</v>
+      </c>
+      <c r="BD8" t="str">
+        <v>-</v>
+      </c>
+      <c r="BE8" t="str">
+        <v>-</v>
+      </c>
+      <c r="BF8" t="str">
+        <v>-</v>
+      </c>
+      <c r="BG8" t="str">
+        <v>-</v>
+      </c>
+      <c r="BH8" t="str">
+        <v>-</v>
+      </c>
+      <c r="BI8" t="str">
+        <v>-</v>
+      </c>
+      <c r="BJ8" t="str">
+        <v>-</v>
+      </c>
+      <c r="BK8" t="str">
+        <v>-</v>
+      </c>
+      <c r="BL8" t="str">
+        <v>-</v>
+      </c>
+      <c r="BM8" t="str">
+        <v>-</v>
+      </c>
+      <c r="BN8" t="str">
+        <v>-</v>
+      </c>
+      <c r="BO8" t="str">
+        <v>-</v>
+      </c>
+      <c r="BP8" t="str">
+        <v>-</v>
+      </c>
+      <c r="BQ8" t="str">
+        <v>-</v>
+      </c>
+      <c r="BR8" t="str">
+        <v>-</v>
+      </c>
+      <c r="BS8" t="str">
+        <v>-</v>
+      </c>
+      <c r="BT8" t="str">
+        <v>-</v>
+      </c>
+      <c r="BU8" t="str">
+        <v>-</v>
+      </c>
+      <c r="BV8" t="str">
+        <v>-</v>
+      </c>
+      <c r="BW8" t="str">
+        <v>-</v>
+      </c>
+      <c r="BX8" t="str">
+        <v>-</v>
+      </c>
+      <c r="BY8" t="str">
+        <v>-</v>
+      </c>
+      <c r="BZ8" t="str">
+        <v>-</v>
+      </c>
+      <c r="CA8" t="str">
+        <v>-</v>
+      </c>
+      <c r="CB8" t="str">
+        <v>-</v>
+      </c>
+      <c r="CC8" t="str">
+        <v>-</v>
+      </c>
+      <c r="CD8" t="str">
+        <v>-</v>
+      </c>
+      <c r="CE8" t="str">
+        <v>-</v>
+      </c>
+      <c r="CF8" t="str">
+        <v>-</v>
+      </c>
+      <c r="CG8" t="str">
+        <v>-</v>
+      </c>
+      <c r="CH8" t="str">
+        <v>-</v>
+      </c>
+      <c r="CI8" t="str">
+        <v>-</v>
+      </c>
+      <c r="CJ8" t="str">
+        <v>-</v>
+      </c>
+      <c r="CK8" t="str">
+        <v>-</v>
+      </c>
+      <c r="CL8" t="str">
+        <v>-</v>
+      </c>
+      <c r="CM8" t="str">
+        <v>-</v>
+      </c>
+      <c r="CN8" t="str">
+        <v>-</v>
+      </c>
+      <c r="CO8" t="str">
+        <v>-</v>
+      </c>
+      <c r="CP8" t="str">
+        <v>-</v>
+      </c>
+      <c r="CQ8" t="str">
+        <v>-</v>
+      </c>
+      <c r="CR8" t="str">
+        <v>-</v>
+      </c>
+      <c r="CS8" t="str">
+        <v>-</v>
+      </c>
+      <c r="CT8" t="str">
+        <v>-</v>
+      </c>
+      <c r="CU8" t="str">
+        <v>-</v>
+      </c>
+      <c r="CV8" t="str">
+        <v>-</v>
+      </c>
+      <c r="CW8" t="str">
+        <v>-</v>
+      </c>
+      <c r="CX8" t="str">
+        <v>-</v>
+      </c>
+      <c r="CY8" t="str">
+        <v>-</v>
+      </c>
+      <c r="CZ8" t="str">
+        <v>-</v>
+      </c>
+      <c r="DA8" t="str">
+        <v>-</v>
+      </c>
+      <c r="DB8" t="str">
+        <v>-</v>
+      </c>
+      <c r="DC8" t="str">
+        <v>-</v>
+      </c>
+      <c r="DD8" t="str">
+        <v>-</v>
+      </c>
+      <c r="DE8" t="str">
+        <v>-</v>
+      </c>
+      <c r="DF8" t="str">
+        <v>-</v>
+      </c>
+      <c r="DG8" t="str">
+        <v>-</v>
+      </c>
+      <c r="DH8" t="str">
+        <v>-</v>
+      </c>
+      <c r="DI8" t="str">
+        <v>-</v>
+      </c>
+      <c r="DJ8" t="str">
+        <v>-</v>
+      </c>
+      <c r="DK8" t="str">
+        <v>-</v>
+      </c>
+      <c r="DL8" t="str">
+        <v>-</v>
+      </c>
+      <c r="DM8" t="str">
+        <v>-</v>
+      </c>
+      <c r="DN8" t="str">
+        <v>-</v>
+      </c>
+      <c r="DO8" t="str">
+        <v>-</v>
+      </c>
+      <c r="DP8" t="str">
+        <v>-</v>
+      </c>
+      <c r="DQ8" t="str">
+        <v>-</v>
+      </c>
+      <c r="DR8" t="str">
+        <v>Aaftab Gill</v>
+      </c>
+      <c r="DS8">
+        <v>43986</v>
+      </c>
+      <c r="DT8" t="str">
+        <v>-</v>
+      </c>
+      <c r="DU8" t="str">
+        <v>yes</v>
+      </c>
+      <c r="DV8" t="str">
+        <v>no</v>
+      </c>
+      <c r="DW8" t="str">
+        <v>yes</v>
+      </c>
+      <c r="DX8" t="str">
+        <v>yes</v>
+      </c>
+      <c r="DY8" t="str">
+        <v>no</v>
+      </c>
+      <c r="DZ8" t="str">
+        <v>yes</v>
+      </c>
+      <c r="EA8" t="str">
+        <v>yes</v>
+      </c>
+      <c r="EB8" t="str">
+        <v>yes</v>
+      </c>
+      <c r="EC8" t="str">
+        <v>yes</v>
+      </c>
+      <c r="ED8" t="str">
+        <v>yes</v>
+      </c>
+      <c r="EE8" t="str">
+        <v>-</v>
+      </c>
+      <c r="EF8" t="str">
+        <v>-</v>
+      </c>
+      <c r="EG8" t="str">
+        <v>-</v>
+      </c>
+      <c r="EH8" t="str">
+        <v>-</v>
+      </c>
+      <c r="EI8" t="str">
+        <v>-</v>
+      </c>
+      <c r="EJ8" t="str">
+        <v>-</v>
+      </c>
+      <c r="EK8" t="str">
+        <v>-</v>
+      </c>
+      <c r="EL8" t="str">
+        <v>-</v>
+      </c>
+      <c r="EM8" t="str">
+        <v>1564 US HIGHWAY 130</v>
+      </c>
+      <c r="EN8" t="str">
+        <v>NORTH BRUNSWICK TOWNSHIP</v>
+      </c>
+      <c r="EO8" t="str">
+        <v>NJ</v>
+      </c>
+      <c r="EP8">
+        <v>8902</v>
+      </c>
+      <c r="EQ8" t="str">
+        <v>-</v>
+      </c>
+      <c r="ER8" t="str">
+        <v>-</v>
+      </c>
+      <c r="ES8" t="str">
+        <v>-</v>
+      </c>
+      <c r="ET8" t="str">
+        <v>-</v>
+      </c>
+      <c r="EU8" t="str">
+        <v>-</v>
+      </c>
+      <c r="EV8" t="str">
+        <v>-</v>
+      </c>
+      <c r="EW8" t="str">
+        <v>-</v>
+      </c>
+      <c r="EX8" t="str">
+        <v>-</v>
+      </c>
+      <c r="EY8" t="str">
+        <v>-</v>
+      </c>
+      <c r="EZ8" t="str">
+        <v>-</v>
+      </c>
+      <c r="FA8" t="str">
+        <v>-</v>
+      </c>
+      <c r="FB8" t="str">
+        <v>-</v>
+      </c>
+      <c r="FC8" t="str">
+        <v>-</v>
+      </c>
+      <c r="FD8" t="str">
+        <v>-</v>
+      </c>
+      <c r="FE8" t="str">
+        <v>-</v>
+      </c>
+      <c r="FF8" t="str">
+        <v>-</v>
+      </c>
+      <c r="FG8" t="str">
+        <v>860-388-4433</v>
+      </c>
+      <c r="FH8" t="str">
+        <v>gilldentalllc@gmail.com</v>
+      </c>
+      <c r="FI8" t="str">
+        <v>-</v>
+      </c>
+      <c r="FJ8" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>3432170909</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Abate</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Martin</v>
+      </c>
+      <c r="D9" t="str">
+        <v>-</v>
+      </c>
+      <c r="E9">
+        <v>33951</v>
+      </c>
+      <c r="F9" t="str">
+        <v>-</v>
+      </c>
+      <c r="G9" t="str">
+        <v>Dentist</v>
+      </c>
+      <c r="H9">
+        <v>1932302106</v>
+      </c>
+      <c r="I9" t="str">
+        <v>MARTIN SCOTT ABATE</v>
+      </c>
+      <c r="J9" t="str">
+        <v>-</v>
+      </c>
+      <c r="K9" t="str">
+        <v>-</v>
+      </c>
+      <c r="L9" t="str">
+        <v>-</v>
+      </c>
+      <c r="M9" t="str">
+        <v>-</v>
+      </c>
+      <c r="N9" t="str">
+        <v>-</v>
+      </c>
+      <c r="O9" t="str">
+        <v>-</v>
+      </c>
+      <c r="P9" t="str">
+        <v>-</v>
+      </c>
+      <c r="Q9" t="str">
+        <v>CLEAN</v>
+      </c>
+      <c r="R9" t="str">
+        <v>07/09/2020</v>
+      </c>
+      <c r="S9" t="str">
+        <v>-</v>
+      </c>
+      <c r="T9" t="str">
+        <v>-</v>
+      </c>
+      <c r="U9">
+        <v>37767</v>
+      </c>
+      <c r="V9" t="str">
+        <v>california</v>
+      </c>
+      <c r="W9" t="str">
+        <v>ABATE, MARTIN SCOTT</v>
+      </c>
+      <c r="X9" t="str">
+        <v>October 31, 2020</v>
+      </c>
+      <c r="Y9" t="str">
+        <v>Current - Active</v>
+      </c>
+      <c r="Z9" t="str">
+        <v>No</v>
+      </c>
+      <c r="AA9" t="str">
+        <v>07/09/2020</v>
+      </c>
+      <c r="AB9" t="str">
+        <v>-</v>
+      </c>
+      <c r="AC9" t="str">
+        <v>-</v>
+      </c>
+      <c r="AD9" t="str">
+        <v>-</v>
+      </c>
+      <c r="AE9" t="str">
+        <v>-</v>
+      </c>
+      <c r="AF9" t="str">
+        <v>-</v>
+      </c>
+      <c r="AG9" t="str">
+        <v>-</v>
+      </c>
+      <c r="AH9" t="str">
+        <v>-</v>
+      </c>
+      <c r="AI9" t="str">
+        <v>-</v>
+      </c>
+      <c r="AJ9" t="str">
+        <v>-</v>
+      </c>
+      <c r="AK9" t="str">
+        <v>-</v>
+      </c>
+      <c r="AL9" t="str">
+        <v>-</v>
+      </c>
+      <c r="AM9" t="str">
+        <v>-</v>
+      </c>
+      <c r="AN9" t="str">
+        <v>-</v>
+      </c>
+      <c r="AO9" t="str">
+        <v>-</v>
+      </c>
+      <c r="AP9" t="str">
+        <v>-</v>
+      </c>
+      <c r="AQ9" t="str">
+        <v>-</v>
+      </c>
+      <c r="AR9" t="str">
+        <v>-</v>
+      </c>
+      <c r="AS9" t="str">
+        <v>-</v>
+      </c>
+      <c r="AT9" t="str">
+        <v>-</v>
+      </c>
+      <c r="AU9" t="str">
+        <v>-</v>
+      </c>
+      <c r="AV9" t="str">
+        <v>-</v>
+      </c>
+      <c r="AW9" t="str">
+        <v>-</v>
+      </c>
+      <c r="AX9" t="str">
+        <v>-</v>
+      </c>
+      <c r="AY9" t="str">
+        <v>-</v>
+      </c>
+      <c r="AZ9" t="str">
+        <v>-</v>
+      </c>
+      <c r="BA9" t="str">
+        <v>-</v>
+      </c>
+      <c r="BB9" t="str">
+        <v>-</v>
+      </c>
+      <c r="BC9" t="str">
+        <v>-</v>
+      </c>
+      <c r="BD9" t="str">
+        <v>-</v>
+      </c>
+      <c r="BE9" t="str">
+        <v>-</v>
+      </c>
+      <c r="BF9" t="str">
+        <v>-</v>
+      </c>
+      <c r="BG9" t="str">
+        <v>-</v>
+      </c>
+      <c r="BH9" t="str">
+        <v>-</v>
+      </c>
+      <c r="BI9" t="str">
+        <v>-</v>
+      </c>
+      <c r="BJ9" t="str">
+        <v>-</v>
+      </c>
+      <c r="BK9" t="str">
+        <v>-</v>
+      </c>
+      <c r="BL9" t="str">
+        <v>-</v>
+      </c>
+      <c r="BM9" t="str">
+        <v>-</v>
+      </c>
+      <c r="BN9" t="str">
+        <v>-</v>
+      </c>
+      <c r="BO9" t="str">
+        <v>-</v>
+      </c>
+      <c r="BP9" t="str">
+        <v>-</v>
+      </c>
+      <c r="BQ9" t="str">
+        <v>-</v>
+      </c>
+      <c r="BR9" t="str">
+        <v>-</v>
+      </c>
+      <c r="BS9" t="str">
+        <v>-</v>
+      </c>
+      <c r="BT9" t="str">
+        <v>-</v>
+      </c>
+      <c r="BU9" t="str">
+        <v>-</v>
+      </c>
+      <c r="BV9" t="str">
+        <v>-</v>
+      </c>
+      <c r="BW9" t="str">
+        <v>-</v>
+      </c>
+      <c r="BX9" t="str">
+        <v>-</v>
+      </c>
+      <c r="BY9" t="str">
+        <v>-</v>
+      </c>
+      <c r="BZ9" t="str">
+        <v>-</v>
+      </c>
+      <c r="CA9" t="str">
+        <v>-</v>
+      </c>
+      <c r="CB9" t="str">
+        <v>-</v>
+      </c>
+      <c r="CC9" t="str">
+        <v>-</v>
+      </c>
+      <c r="CD9" t="str">
+        <v>-</v>
+      </c>
+      <c r="CE9" t="str">
+        <v>-</v>
+      </c>
+      <c r="CF9" t="str">
+        <v>-</v>
+      </c>
+      <c r="CG9" t="str">
+        <v>-</v>
+      </c>
+      <c r="CH9" t="str">
+        <v>-</v>
+      </c>
+      <c r="CI9" t="str">
+        <v>-</v>
+      </c>
+      <c r="CJ9" t="str">
+        <v>-</v>
+      </c>
+      <c r="CK9" t="str">
+        <v>-</v>
+      </c>
+      <c r="CL9" t="str">
+        <v>-</v>
+      </c>
+      <c r="CM9" t="str">
+        <v>-</v>
+      </c>
+      <c r="CN9" t="str">
+        <v>-</v>
+      </c>
+      <c r="CO9" t="str">
+        <v>-</v>
+      </c>
+      <c r="CP9" t="str">
+        <v>-</v>
+      </c>
+      <c r="CQ9" t="str">
+        <v>-</v>
+      </c>
+      <c r="CR9" t="str">
+        <v>-</v>
+      </c>
+      <c r="CS9" t="str">
+        <v>-</v>
+      </c>
+      <c r="CT9" t="str">
+        <v>-</v>
+      </c>
+      <c r="CU9" t="str">
+        <v>-</v>
+      </c>
+      <c r="CV9" t="str">
+        <v>-</v>
+      </c>
+      <c r="CW9" t="str">
+        <v>-</v>
+      </c>
+      <c r="CX9" t="str">
+        <v>-</v>
+      </c>
+      <c r="CY9" t="str">
+        <v>-</v>
+      </c>
+      <c r="CZ9" t="str">
+        <v>-</v>
+      </c>
+      <c r="DA9" t="str">
+        <v>-</v>
+      </c>
+      <c r="DB9" t="str">
+        <v>-</v>
+      </c>
+      <c r="DC9" t="str">
+        <v>-</v>
+      </c>
+      <c r="DD9" t="str">
+        <v>-</v>
+      </c>
+      <c r="DE9" t="str">
+        <v>-</v>
+      </c>
+      <c r="DF9" t="str">
+        <v>-</v>
+      </c>
+      <c r="DG9" t="str">
+        <v>-</v>
+      </c>
+      <c r="DH9" t="str">
+        <v>-</v>
+      </c>
+      <c r="DI9" t="str">
+        <v>-</v>
+      </c>
+      <c r="DJ9" t="str">
+        <v>-</v>
+      </c>
+      <c r="DK9" t="str">
+        <v>-</v>
+      </c>
+      <c r="DL9" t="str">
+        <v>-</v>
+      </c>
+      <c r="DM9" t="str">
+        <v>-</v>
+      </c>
+      <c r="DN9" t="str">
+        <v>-</v>
+      </c>
+      <c r="DO9" t="str">
+        <v>-</v>
+      </c>
+      <c r="DP9" t="str">
+        <v>-</v>
+      </c>
+      <c r="DQ9" t="str">
+        <v>-</v>
+      </c>
+      <c r="DR9" t="str">
+        <v>Martin S. Abate</v>
+      </c>
+      <c r="DS9">
+        <v>43952</v>
+      </c>
+      <c r="DT9" t="str">
+        <v>-</v>
+      </c>
+      <c r="DU9" t="str">
+        <v>yes</v>
+      </c>
+      <c r="DV9" t="str">
+        <v>yes</v>
+      </c>
+      <c r="DW9" t="str">
+        <v>no</v>
+      </c>
+      <c r="DX9" t="str">
+        <v>yes</v>
+      </c>
+      <c r="DY9" t="str">
+        <v>yes</v>
+      </c>
+      <c r="DZ9" t="str">
+        <v>yes</v>
+      </c>
+      <c r="EA9" t="str">
+        <v>yes</v>
+      </c>
+      <c r="EB9" t="str">
+        <v>yes</v>
+      </c>
+      <c r="EC9" t="str">
+        <v>yes</v>
+      </c>
+      <c r="ED9" t="str">
+        <v>yes</v>
+      </c>
+      <c r="EE9" t="str">
+        <v>-</v>
+      </c>
+      <c r="EF9" t="str">
+        <v>-</v>
+      </c>
+      <c r="EG9" t="str">
+        <v>-</v>
+      </c>
+      <c r="EH9" t="str">
+        <v>-</v>
+      </c>
+      <c r="EI9" t="str">
+        <v>-</v>
+      </c>
+      <c r="EJ9" t="str">
+        <v>-</v>
+      </c>
+      <c r="EK9" t="str">
+        <v>-</v>
+      </c>
+      <c r="EL9" t="str">
+        <v>-</v>
+      </c>
+      <c r="EM9" t="str">
+        <v>3637 SACRAMENTO ST</v>
+      </c>
+      <c r="EN9" t="str">
+        <v>SAN FRANCISCO</v>
+      </c>
+      <c r="EO9" t="str">
+        <v>CA</v>
+      </c>
+      <c r="EP9">
+        <v>94118</v>
+      </c>
+      <c r="EQ9" t="str">
+        <v>-</v>
+      </c>
+      <c r="ER9" t="str">
+        <v>-</v>
+      </c>
+      <c r="ES9" t="str">
+        <v>-</v>
+      </c>
+      <c r="ET9" t="str">
+        <v>-</v>
+      </c>
+      <c r="EU9" t="str">
+        <v>-</v>
+      </c>
+      <c r="EV9" t="str">
+        <v>-</v>
+      </c>
+      <c r="EW9" t="str">
+        <v>-</v>
+      </c>
+      <c r="EX9" t="str">
+        <v>-</v>
+      </c>
+      <c r="EY9" t="str">
+        <v>-</v>
+      </c>
+      <c r="EZ9" t="str">
+        <v>-</v>
+      </c>
+      <c r="FA9" t="str">
+        <v>-</v>
+      </c>
+      <c r="FB9" t="str">
+        <v>-</v>
+      </c>
+      <c r="FC9" t="str">
+        <v>-</v>
+      </c>
+      <c r="FD9" t="str">
+        <v>-</v>
+      </c>
+      <c r="FE9" t="str">
+        <v>-</v>
+      </c>
+      <c r="FF9" t="str">
+        <v>-</v>
+      </c>
+      <c r="FG9" t="str">
+        <v>415-989-1001</v>
+      </c>
+      <c r="FH9" t="str">
+        <v>martin.abate@gmail.com</v>
+      </c>
+      <c r="FI9" t="str">
+        <v>-</v>
+      </c>
+      <c r="FJ9" t="str">
+        <v>No -Cannot set headers after they are sent to the client</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:FI5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:FJ9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>